<commit_message>
GDE-9313 After addressing comments 12DEC2020
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -1335,10 +1335,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CM2"/>
+  <dimension ref="A1:CQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BE1" sqref="BE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1387,8 +1387,12 @@
     <col width="34.140625" bestFit="1" customWidth="1" style="27" min="51" max="51"/>
     <col width="28.42578125" bestFit="1" customWidth="1" style="27" min="52" max="52"/>
     <col width="11.140625" bestFit="1" customWidth="1" style="27" min="53" max="53"/>
-    <col width="15.28515625" bestFit="1" customWidth="1" style="27" min="54" max="55"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="27" min="89" max="89"/>
+    <col width="23.7109375" bestFit="1" customWidth="1" style="27" min="54" max="54"/>
+    <col width="28.28515625" bestFit="1" customWidth="1" style="27" min="55" max="55"/>
+    <col width="28.28515625" customWidth="1" style="27" min="56" max="56"/>
+    <col width="23.7109375" customWidth="1" style="27" min="57" max="57"/>
+    <col width="15.28515625" bestFit="1" customWidth="1" style="27" min="58" max="59"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="27" min="93" max="93"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="24">
@@ -1659,190 +1663,210 @@
       </c>
       <c r="BB1" s="24" t="inlineStr">
         <is>
+          <t>Ratios_And_Cons_Index</t>
+        </is>
+      </c>
+      <c r="BC1" s="24" t="inlineStr">
+        <is>
+          <t>Ratios_And_Cons_Description</t>
+        </is>
+      </c>
+      <c r="BD1" s="24" t="inlineStr">
+        <is>
+          <t>Ratios_And_Cons_StartDate</t>
+        </is>
+      </c>
+      <c r="BE1" s="24" t="inlineStr">
+        <is>
+          <t>Ratios_And_Cons_RadioButton</t>
+        </is>
+      </c>
+      <c r="BF1" s="24" t="inlineStr">
+        <is>
           <t>Financial_Ratio</t>
         </is>
       </c>
-      <c r="BC1" s="24" t="inlineStr">
+      <c r="BG1" s="24" t="inlineStr">
         <is>
           <t>Ratio_StartDate</t>
         </is>
       </c>
-      <c r="BD1" s="24" t="inlineStr">
+      <c r="BH1" s="24" t="inlineStr">
         <is>
           <t>BankRole_Type</t>
         </is>
       </c>
-      <c r="BE1" s="24" t="inlineStr">
+      <c r="BI1" s="24" t="inlineStr">
         <is>
           <t>Reference_Bank</t>
         </is>
       </c>
-      <c r="BF1" s="24" t="inlineStr">
+      <c r="BJ1" s="24" t="inlineStr">
         <is>
           <t>Bid_Bank</t>
         </is>
       </c>
-      <c r="BG1" s="24" t="inlineStr">
+      <c r="BK1" s="24" t="inlineStr">
         <is>
           <t>SBLC_Issuer</t>
         </is>
       </c>
-      <c r="BH1" s="24" t="inlineStr">
+      <c r="BL1" s="24" t="inlineStr">
         <is>
           <t>Swingline_Bank</t>
         </is>
       </c>
-      <c r="BI1" s="24" t="inlineStr">
+      <c r="BM1" s="24" t="inlineStr">
         <is>
           <t>BA_Issuing_Bank</t>
         </is>
       </c>
-      <c r="BJ1" s="24" t="inlineStr">
+      <c r="BN1" s="24" t="inlineStr">
         <is>
           <t>BA_Reference_Bank</t>
         </is>
       </c>
-      <c r="BK1" s="24" t="inlineStr">
+      <c r="BO1" s="24" t="inlineStr">
         <is>
           <t>BA_Owner_Bank</t>
         </is>
       </c>
-      <c r="BL1" s="24" t="inlineStr">
+      <c r="BP1" s="24" t="inlineStr">
         <is>
           <t>RAC_Reference_Bank</t>
         </is>
       </c>
-      <c r="BM1" s="24" t="inlineStr">
+      <c r="BQ1" s="24" t="inlineStr">
         <is>
           <t>BankRole_Percent</t>
         </is>
       </c>
-      <c r="BN1" s="24" t="inlineStr">
+      <c r="BR1" s="24" t="inlineStr">
         <is>
           <t>BankRole_BankName</t>
         </is>
       </c>
-      <c r="BO1" s="24" t="inlineStr">
+      <c r="BS1" s="24" t="inlineStr">
         <is>
           <t>BankRole_SGAlias</t>
         </is>
       </c>
-      <c r="BP1" s="24" t="inlineStr">
+      <c r="BT1" s="24" t="inlineStr">
         <is>
           <t>BankRole_SGContactName</t>
         </is>
       </c>
-      <c r="BQ1" s="24" t="inlineStr">
+      <c r="BU1" s="24" t="inlineStr">
         <is>
           <t>BankRole_SGRIMethod</t>
         </is>
       </c>
-      <c r="BR1" s="24" t="inlineStr">
+      <c r="BV1" s="24" t="inlineStr">
         <is>
           <t>BankRole_SGName</t>
         </is>
       </c>
-      <c r="BS1" s="24" t="inlineStr">
+      <c r="BW1" s="24" t="inlineStr">
         <is>
           <t>BankRole_Portfolio</t>
         </is>
       </c>
-      <c r="BT1" s="24" t="inlineStr">
+      <c r="BX1" s="24" t="inlineStr">
         <is>
           <t>BankRole_ExpenseCode</t>
         </is>
       </c>
-      <c r="BU1" s="24" t="inlineStr">
+      <c r="BY1" s="24" t="inlineStr">
         <is>
           <t>BankRole_ExpenseCodeDesc</t>
         </is>
       </c>
-      <c r="BV1" s="24" t="inlineStr">
+      <c r="BZ1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_IncomeMethod</t>
         </is>
       </c>
-      <c r="BW1" s="24" t="inlineStr">
+      <c r="CA1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_AmountType</t>
         </is>
       </c>
-      <c r="BX1" s="24" t="inlineStr">
+      <c r="CB1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_Amount</t>
         </is>
       </c>
-      <c r="BY1" s="24" t="inlineStr">
+      <c r="CC1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_EffectiveDate</t>
         </is>
       </c>
-      <c r="BZ1" s="24" t="inlineStr">
+      <c r="CD1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_Frequency</t>
         </is>
       </c>
-      <c r="CA1" s="24" t="inlineStr">
+      <c r="CE1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_Customer</t>
         </is>
       </c>
-      <c r="CB1" s="24" t="inlineStr">
+      <c r="CF1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_CustomerLocation</t>
         </is>
       </c>
-      <c r="CC1" s="24" t="inlineStr">
+      <c r="CG1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_ExpenseCode</t>
         </is>
       </c>
-      <c r="CD1" s="24" t="inlineStr">
+      <c r="CH1" s="24" t="inlineStr">
         <is>
           <t>AdminFee_PercentOfFee</t>
         </is>
       </c>
-      <c r="CE1" s="24" t="inlineStr">
+      <c r="CI1" s="24" t="inlineStr">
         <is>
           <t>UpfrontFee_Category</t>
         </is>
       </c>
-      <c r="CF1" s="24" t="inlineStr">
+      <c r="CJ1" s="24" t="inlineStr">
         <is>
           <t>UpfrontFee_Type</t>
         </is>
       </c>
-      <c r="CG1" s="24" t="inlineStr">
+      <c r="CK1" s="24" t="inlineStr">
         <is>
           <t>UpfrontFee_RateBasis</t>
         </is>
       </c>
-      <c r="CH1" s="24" t="inlineStr">
+      <c r="CL1" s="24" t="inlineStr">
         <is>
           <t>UpfrontFee_Amount</t>
         </is>
       </c>
-      <c r="CI1" s="24" t="inlineStr">
+      <c r="CM1" s="24" t="inlineStr">
         <is>
           <t>UpfrontFeePayment_Comment</t>
         </is>
       </c>
-      <c r="CJ1" s="24" t="inlineStr">
+      <c r="CN1" s="24" t="inlineStr">
         <is>
           <t>EstablishmentFee_EffectiveDate</t>
         </is>
       </c>
-      <c r="CK1" s="24" t="inlineStr">
+      <c r="CO1" s="24" t="inlineStr">
         <is>
           <t>Deal_SalesGroup</t>
         </is>
       </c>
-      <c r="CL1" s="24" t="inlineStr">
+      <c r="CP1" s="24" t="inlineStr">
         <is>
           <t>Borrower_PreferredRIMthd1</t>
         </is>
       </c>
-      <c r="CM1" s="24" t="inlineStr">
+      <c r="CQ1" s="24" t="inlineStr">
         <is>
           <t>Borrower_RemittanceDescription</t>
         </is>
@@ -1866,7 +1890,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_18112</t>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_56120</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2044,7 +2068,25 @@
           <t>Next Business Day</t>
         </is>
       </c>
-      <c r="CK2" t="inlineStr">
+      <c r="BB2" s="28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BC2" s="8" t="inlineStr">
+        <is>
+          <t>average unfunded committed account &gt;40%</t>
+        </is>
+      </c>
+      <c r="BD2" s="8" t="n">
+        <v>42266</v>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="CO2" t="inlineStr">
         <is>
           <t>Sales Group 1</t>
         </is>
@@ -2290,7 +2332,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_18112</t>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_56120</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -2498,7 +2540,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_18112</t>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_56120</t>
         </is>
       </c>
     </row>
@@ -2639,7 +2681,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_18112</t>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_56120</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-9314 -Added initial drawdown -updated xls for drawdown -added ticking of reference banks apply checkbox and intent notice days in advance in deal creation
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_CommitmentFeePayment" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SYND02_PrimaryAllocation" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Correspondence" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -21,11 +22,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
     <numFmt numFmtId="165" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="166" formatCode="00000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -89,13 +91,6 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <sz val="11"/>
     </font>
     <font>
@@ -123,7 +118,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill/>
     </fill>
@@ -190,6 +185,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -221,7 +234,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -289,16 +302,14 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -309,7 +320,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -322,10 +333,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,172 +791,172 @@
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="49" t="inlineStr">
+      <c r="C1" s="47" t="inlineStr">
         <is>
           <t>Enterprise_Prefix</t>
         </is>
       </c>
-      <c r="D1" s="51" t="inlineStr">
+      <c r="D1" s="49" t="inlineStr">
         <is>
           <t>Party_ID</t>
         </is>
       </c>
-      <c r="E1" s="49" t="inlineStr">
+      <c r="E1" s="47" t="inlineStr">
         <is>
           <t>Short_Name_Prefix</t>
         </is>
       </c>
-      <c r="F1" s="49" t="inlineStr">
+      <c r="F1" s="47" t="inlineStr">
         <is>
           <t>Locality</t>
         </is>
       </c>
-      <c r="G1" s="49" t="inlineStr">
+      <c r="G1" s="47" t="inlineStr">
         <is>
           <t>Branch_Code</t>
         </is>
       </c>
-      <c r="H1" s="49" t="inlineStr">
+      <c r="H1" s="47" t="inlineStr">
         <is>
           <t>Party_Type</t>
         </is>
       </c>
-      <c r="I1" s="49" t="inlineStr">
+      <c r="I1" s="47" t="inlineStr">
         <is>
           <t>Party_Sub_Type</t>
         </is>
       </c>
-      <c r="J1" s="49" t="inlineStr">
+      <c r="J1" s="47" t="inlineStr">
         <is>
           <t>Party_Category</t>
         </is>
       </c>
-      <c r="K1" s="49" t="inlineStr">
+      <c r="K1" s="47" t="inlineStr">
         <is>
           <t>Registered_Number</t>
         </is>
       </c>
-      <c r="L1" s="49" t="inlineStr">
+      <c r="L1" s="47" t="inlineStr">
         <is>
           <t>Country_of_Tax_Domicile</t>
         </is>
       </c>
-      <c r="M1" s="49" t="inlineStr">
+      <c r="M1" s="47" t="inlineStr">
         <is>
           <t>Country_of_Registration</t>
         </is>
       </c>
-      <c r="N1" s="49" t="inlineStr">
+      <c r="N1" s="47" t="inlineStr">
         <is>
           <t>Business_Country</t>
         </is>
       </c>
-      <c r="O1" s="49" t="inlineStr">
+      <c r="O1" s="47" t="inlineStr">
         <is>
           <t>Industry_Sector</t>
         </is>
       </c>
-      <c r="P1" s="49" t="inlineStr">
+      <c r="P1" s="47" t="inlineStr">
         <is>
           <t>Business_Activity</t>
         </is>
       </c>
-      <c r="Q1" s="49" t="inlineStr">
+      <c r="Q1" s="47" t="inlineStr">
         <is>
           <t>Is_Main_Activity</t>
         </is>
       </c>
-      <c r="R1" s="49" t="inlineStr">
+      <c r="R1" s="47" t="inlineStr">
         <is>
           <t>Is_Primary_Activity</t>
         </is>
       </c>
-      <c r="S1" s="49" t="inlineStr">
+      <c r="S1" s="47" t="inlineStr">
         <is>
           <t>GST_Number</t>
         </is>
       </c>
-      <c r="T1" s="49" t="inlineStr">
+      <c r="T1" s="47" t="inlineStr">
         <is>
           <t>Address_Type</t>
         </is>
       </c>
-      <c r="U1" s="49" t="inlineStr">
+      <c r="U1" s="47" t="inlineStr">
         <is>
           <t>Country_Region</t>
         </is>
       </c>
-      <c r="V1" s="49" t="inlineStr">
+      <c r="V1" s="47" t="inlineStr">
         <is>
           <t>Post_Code</t>
         </is>
       </c>
-      <c r="W1" s="49" t="inlineStr">
+      <c r="W1" s="47" t="inlineStr">
         <is>
           <t>Address_Line_1</t>
         </is>
       </c>
-      <c r="X1" s="49" t="inlineStr">
+      <c r="X1" s="47" t="inlineStr">
         <is>
           <t>Address_Line_2</t>
         </is>
       </c>
-      <c r="Y1" s="49" t="inlineStr">
+      <c r="Y1" s="47" t="inlineStr">
         <is>
           <t>Address_Line_3</t>
         </is>
       </c>
-      <c r="Z1" s="49" t="inlineStr">
+      <c r="Z1" s="47" t="inlineStr">
         <is>
           <t>Address_Line_4</t>
         </is>
       </c>
-      <c r="AA1" s="49" t="inlineStr">
+      <c r="AA1" s="47" t="inlineStr">
         <is>
           <t>Town_City</t>
         </is>
       </c>
-      <c r="AB1" s="49" t="inlineStr">
+      <c r="AB1" s="47" t="inlineStr">
         <is>
           <t>State_Province</t>
         </is>
       </c>
-      <c r="AC1" s="49" t="inlineStr">
+      <c r="AC1" s="47" t="inlineStr">
         <is>
           <t>Document_Collection_Status</t>
         </is>
       </c>
-      <c r="AD1" s="49" t="inlineStr">
+      <c r="AD1" s="47" t="inlineStr">
         <is>
           <t>Selected_Module</t>
         </is>
       </c>
-      <c r="AE1" s="49" t="inlineStr">
+      <c r="AE1" s="47" t="inlineStr">
         <is>
           <t>UserZone</t>
         </is>
       </c>
-      <c r="AF1" s="49" t="inlineStr">
+      <c r="AF1" s="47" t="inlineStr">
         <is>
           <t>UserBranch</t>
         </is>
       </c>
-      <c r="AG1" s="49" t="inlineStr">
+      <c r="AG1" s="47" t="inlineStr">
         <is>
           <t>CustomerNotice_TypeMethod</t>
         </is>
       </c>
-      <c r="AH1" s="49" t="inlineStr">
+      <c r="AH1" s="47" t="inlineStr">
         <is>
           <t>Expense_Code</t>
         </is>
       </c>
-      <c r="AI1" s="49" t="inlineStr">
+      <c r="AI1" s="47" t="inlineStr">
         <is>
           <t>Deparment_Code</t>
         </is>
       </c>
-      <c r="AJ1" s="49" t="inlineStr">
+      <c r="AJ1" s="47" t="inlineStr">
         <is>
           <t>Profile_Type</t>
         </is>
@@ -908,152 +976,152 @@
           <t>LIQBorrower_LegalName</t>
         </is>
       </c>
-      <c r="AN1" s="51" t="inlineStr">
+      <c r="AN1" s="49" t="inlineStr">
         <is>
           <t>LIQCustomer_ShortName</t>
         </is>
       </c>
-      <c r="AO1" s="49" t="inlineStr">
+      <c r="AO1" s="47" t="inlineStr">
         <is>
           <t>Contact_FirstName</t>
         </is>
       </c>
-      <c r="AP1" s="49" t="inlineStr">
+      <c r="AP1" s="47" t="inlineStr">
         <is>
           <t>Contact_LastName</t>
         </is>
       </c>
-      <c r="AQ1" s="49" t="inlineStr">
+      <c r="AQ1" s="47" t="inlineStr">
         <is>
           <t>Contact_PreferredLanguage</t>
         </is>
       </c>
-      <c r="AR1" s="49" t="inlineStr">
+      <c r="AR1" s="47" t="inlineStr">
         <is>
           <t>Contact_PrimaryPhone</t>
         </is>
       </c>
-      <c r="AS1" s="49" t="inlineStr">
+      <c r="AS1" s="47" t="inlineStr">
         <is>
           <t>BorrowerContact_Phone</t>
         </is>
       </c>
-      <c r="AT1" s="49" t="inlineStr">
+      <c r="AT1" s="47" t="inlineStr">
         <is>
           <t>Contact_PurposeType</t>
         </is>
       </c>
-      <c r="AU1" s="49" t="inlineStr">
+      <c r="AU1" s="47" t="inlineStr">
         <is>
           <t>ContactNotice_Method</t>
         </is>
       </c>
-      <c r="AV1" s="49" t="inlineStr">
+      <c r="AV1" s="47" t="inlineStr">
         <is>
           <t>Contact_Email</t>
         </is>
       </c>
-      <c r="AW1" s="49" t="inlineStr">
+      <c r="AW1" s="47" t="inlineStr">
         <is>
           <t>ProductSBLC_Checkbox</t>
         </is>
       </c>
-      <c r="AX1" s="49" t="inlineStr">
+      <c r="AX1" s="47" t="inlineStr">
         <is>
           <t>ProductLoan_Checkbox</t>
         </is>
       </c>
-      <c r="AY1" s="49" t="inlineStr">
+      <c r="AY1" s="47" t="inlineStr">
         <is>
           <t>BalanceType_Principal_Checkbox</t>
         </is>
       </c>
-      <c r="AZ1" s="49" t="inlineStr">
+      <c r="AZ1" s="47" t="inlineStr">
         <is>
           <t>BalanceType_Interest_Checkbox</t>
         </is>
       </c>
-      <c r="BA1" s="49" t="inlineStr">
+      <c r="BA1" s="47" t="inlineStr">
         <is>
           <t>BalanceType_Fees_Checkbox</t>
         </is>
       </c>
-      <c r="BB1" s="49" t="inlineStr">
+      <c r="BB1" s="47" t="inlineStr">
         <is>
           <t>Address_Code</t>
         </is>
       </c>
-      <c r="BC1" s="49" t="inlineStr">
+      <c r="BC1" s="47" t="inlineStr">
         <is>
           <t>RI_DDAMethod</t>
         </is>
       </c>
-      <c r="BD1" s="49" t="inlineStr">
+      <c r="BD1" s="47" t="inlineStr">
         <is>
           <t>RI_DDADescription</t>
         </is>
       </c>
-      <c r="BE1" s="49" t="inlineStr">
+      <c r="BE1" s="47" t="inlineStr">
         <is>
           <t>RI_DDAAccountName</t>
         </is>
       </c>
-      <c r="BF1" s="49" t="inlineStr">
+      <c r="BF1" s="47" t="inlineStr">
         <is>
           <t>RI_DDAAccountNumber</t>
         </is>
       </c>
-      <c r="BG1" s="49" t="inlineStr">
+      <c r="BG1" s="47" t="inlineStr">
         <is>
           <t>RI_DDACurrency</t>
         </is>
       </c>
-      <c r="BH1" s="49" t="inlineStr">
+      <c r="BH1" s="47" t="inlineStr">
         <is>
           <t>RI_ProductLoan_Checkbox</t>
         </is>
       </c>
-      <c r="BI1" s="49" t="inlineStr">
+      <c r="BI1" s="47" t="inlineStr">
         <is>
           <t>RI_ProductSBLC_Checkbox</t>
         </is>
       </c>
-      <c r="BJ1" s="49" t="inlineStr">
+      <c r="BJ1" s="47" t="inlineStr">
         <is>
           <t>RI_FromCust_Checkbox</t>
         </is>
       </c>
-      <c r="BK1" s="49" t="inlineStr">
+      <c r="BK1" s="47" t="inlineStr">
         <is>
           <t>RI_ToCust_Checkbox</t>
         </is>
       </c>
-      <c r="BL1" s="49" t="inlineStr">
+      <c r="BL1" s="47" t="inlineStr">
         <is>
           <t>RI_BalanceType_Principal_Checkbox</t>
         </is>
       </c>
-      <c r="BM1" s="49" t="inlineStr">
+      <c r="BM1" s="47" t="inlineStr">
         <is>
           <t>RI_BalanceType_Interest_Checkbox</t>
         </is>
       </c>
-      <c r="BN1" s="49" t="inlineStr">
+      <c r="BN1" s="47" t="inlineStr">
         <is>
           <t>RI_BalanceType_Fees_Checkbox</t>
         </is>
       </c>
-      <c r="BO1" s="49" t="inlineStr">
+      <c r="BO1" s="47" t="inlineStr">
         <is>
           <t>RI_AutoDoIt_Checkbox</t>
         </is>
       </c>
-      <c r="BP1" s="49" t="inlineStr">
+      <c r="BP1" s="47" t="inlineStr">
         <is>
           <t>Group_Contact</t>
         </is>
       </c>
-      <c r="BQ1" s="49" t="n"/>
+      <c r="BQ1" s="47" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1413,14 +1481,14 @@
       </c>
     </row>
     <row r="21" customFormat="1" s="8">
-      <c r="C21" s="49" t="inlineStr">
+      <c r="C21" s="47" t="inlineStr">
         <is>
           <t>Manual Input</t>
         </is>
       </c>
     </row>
     <row r="22" customFormat="1" s="8">
-      <c r="C22" s="51" t="inlineStr">
+      <c r="C22" s="49" t="inlineStr">
         <is>
           <t>Auto generated</t>
         </is>
@@ -1452,10 +1520,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CQ2"/>
+  <dimension ref="A1:CS2"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1466,7 +1534,8 @@
     <col width="16.140625" bestFit="1" customWidth="1" style="24" min="4" max="4"/>
     <col width="48.140625" bestFit="1" customWidth="1" style="24" min="5" max="5"/>
     <col width="10.5703125" bestFit="1" customWidth="1" style="24" min="6" max="6"/>
-    <col width="14" bestFit="1" customWidth="1" style="24" min="7" max="7"/>
+    <col width="28.85546875" bestFit="1" customWidth="1" style="24" min="7" max="7"/>
+    <col width="14.42578125" bestFit="1" customWidth="1" style="24" min="8" max="8"/>
     <col width="22.5703125" bestFit="1" customWidth="1" style="24" min="9" max="9"/>
     <col width="21" bestFit="1" customWidth="1" style="24" min="10" max="10"/>
     <col width="36.28515625" bestFit="1" customWidth="1" style="24" min="16" max="16"/>
@@ -1496,495 +1565,506 @@
     <col width="46.85546875" bestFit="1" customWidth="1" style="24" min="42" max="42"/>
     <col width="39.140625" bestFit="1" customWidth="1" style="24" min="43" max="43"/>
     <col width="26.42578125" bestFit="1" customWidth="1" style="24" min="44" max="44"/>
-    <col width="40" bestFit="1" customWidth="1" style="24" min="45" max="45"/>
-    <col width="31.85546875" bestFit="1" customWidth="1" style="24" min="46" max="46"/>
-    <col width="24.85546875" bestFit="1" customWidth="1" style="24" min="47" max="47"/>
-    <col width="25" bestFit="1" customWidth="1" style="24" min="48" max="48"/>
-    <col width="25" customWidth="1" style="24" min="49" max="49"/>
-    <col width="16.140625" bestFit="1" customWidth="1" style="24" min="50" max="50"/>
-    <col width="34.140625" bestFit="1" customWidth="1" style="24" min="51" max="51"/>
-    <col width="28.42578125" bestFit="1" customWidth="1" style="24" min="52" max="52"/>
-    <col width="11.140625" bestFit="1" customWidth="1" style="24" min="53" max="53"/>
-    <col width="23.7109375" bestFit="1" customWidth="1" style="24" min="54" max="54"/>
-    <col width="38.140625" bestFit="1" customWidth="1" style="24" min="55" max="55"/>
-    <col width="28.28515625" customWidth="1" style="24" min="56" max="56"/>
-    <col width="23.7109375" customWidth="1" style="24" min="57" max="57"/>
-    <col width="15.28515625" bestFit="1" customWidth="1" style="24" min="58" max="59"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="24" min="93" max="93"/>
+    <col width="40.42578125" bestFit="1" customWidth="1" style="24" min="45" max="45"/>
+    <col width="40.42578125" customWidth="1" style="24" min="46" max="47"/>
+    <col width="31.85546875" bestFit="1" customWidth="1" style="24" min="48" max="48"/>
+    <col width="24.85546875" bestFit="1" customWidth="1" style="24" min="49" max="49"/>
+    <col width="25" bestFit="1" customWidth="1" style="24" min="50" max="50"/>
+    <col width="25" customWidth="1" style="24" min="51" max="51"/>
+    <col width="16.140625" bestFit="1" customWidth="1" style="24" min="52" max="52"/>
+    <col width="34.140625" bestFit="1" customWidth="1" style="24" min="53" max="53"/>
+    <col width="28.42578125" bestFit="1" customWidth="1" style="24" min="54" max="54"/>
+    <col width="11.140625" bestFit="1" customWidth="1" style="24" min="55" max="55"/>
+    <col width="23.7109375" bestFit="1" customWidth="1" style="24" min="56" max="56"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="24" min="57" max="57"/>
+    <col width="28.28515625" customWidth="1" style="24" min="58" max="58"/>
+    <col width="23.7109375" customWidth="1" style="24" min="59" max="59"/>
+    <col width="15.28515625" bestFit="1" customWidth="1" style="24" min="60" max="61"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="24" min="95" max="95"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customFormat="1" customHeight="1" s="49">
+    <row r="1" ht="12.75" customFormat="1" customHeight="1" s="47">
       <c r="A1" s="23" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="49" t="inlineStr">
+      <c r="B1" s="47" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="49" t="inlineStr">
+      <c r="C1" s="47" t="inlineStr">
         <is>
           <t>Deal_NamePrefix</t>
         </is>
       </c>
-      <c r="D1" s="49" t="inlineStr">
+      <c r="D1" s="47" t="inlineStr">
         <is>
           <t>Deal_AliasPrefix</t>
         </is>
       </c>
-      <c r="E1" s="50" t="inlineStr">
+      <c r="E1" s="48" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="F1" s="50" t="inlineStr">
+      <c r="F1" s="48" t="inlineStr">
         <is>
           <t>Deal_Alias</t>
         </is>
       </c>
-      <c r="G1" s="50" t="inlineStr">
+      <c r="G1" s="48" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="H1" s="49" t="inlineStr">
+      <c r="H1" s="47" t="inlineStr">
         <is>
           <t>Deal_Currency</t>
         </is>
       </c>
-      <c r="I1" s="50" t="inlineStr">
+      <c r="I1" s="48" t="inlineStr">
         <is>
           <t>Borrower_ShortName</t>
         </is>
       </c>
-      <c r="J1" s="51" t="inlineStr">
+      <c r="J1" s="49" t="inlineStr">
         <is>
           <t>Borrower_Location</t>
         </is>
       </c>
-      <c r="K1" s="49" t="inlineStr">
+      <c r="K1" s="47" t="inlineStr">
         <is>
           <t>Borrower_Depositor_Indicator</t>
         </is>
       </c>
-      <c r="L1" s="49" t="inlineStr">
+      <c r="L1" s="47" t="inlineStr">
         <is>
           <t>Borrower_SGAlias</t>
         </is>
       </c>
-      <c r="M1" s="49" t="inlineStr">
+      <c r="M1" s="47" t="inlineStr">
         <is>
           <t>Borrower_SG_Name</t>
         </is>
       </c>
-      <c r="N1" s="49" t="inlineStr">
+      <c r="N1" s="47" t="inlineStr">
         <is>
           <t>Borrower_SG_GroupMembers</t>
         </is>
       </c>
-      <c r="O1" s="49" t="inlineStr">
+      <c r="O1" s="47" t="inlineStr">
         <is>
           <t>Borrower_PreferredRIMthd</t>
         </is>
       </c>
-      <c r="P1" s="49" t="inlineStr">
+      <c r="P1" s="47" t="inlineStr">
         <is>
           <t>Deal_AdminAgent</t>
         </is>
       </c>
-      <c r="Q1" s="49" t="inlineStr">
+      <c r="Q1" s="47" t="inlineStr">
         <is>
           <t>AdminAgent_Location</t>
         </is>
       </c>
-      <c r="R1" s="49" t="inlineStr">
+      <c r="R1" s="47" t="inlineStr">
         <is>
           <t>AdminAgent_SGAlias</t>
         </is>
       </c>
-      <c r="S1" s="49" t="inlineStr">
+      <c r="S1" s="47" t="inlineStr">
         <is>
           <t>AdminAgent_SGName</t>
         </is>
       </c>
-      <c r="T1" s="49" t="inlineStr">
+      <c r="T1" s="47" t="inlineStr">
         <is>
           <t>AdminAgent_ContactName</t>
         </is>
       </c>
-      <c r="U1" s="49" t="inlineStr">
+      <c r="U1" s="47" t="inlineStr">
         <is>
           <t>AdminAgent_RIMethod</t>
         </is>
       </c>
-      <c r="V1" s="49" t="inlineStr">
+      <c r="V1" s="47" t="inlineStr">
         <is>
           <t>Deal_ClassificationCode</t>
         </is>
       </c>
-      <c r="W1" s="49" t="inlineStr">
+      <c r="W1" s="47" t="inlineStr">
         <is>
           <t>Deal_ClassificationDesc</t>
         </is>
       </c>
-      <c r="X1" s="49" t="inlineStr">
+      <c r="X1" s="47" t="inlineStr">
         <is>
           <t>Deal_AgreementDate</t>
         </is>
       </c>
-      <c r="Y1" s="49" t="inlineStr">
+      <c r="Y1" s="47" t="inlineStr">
         <is>
           <t>Deal_ApprovedDate</t>
         </is>
       </c>
-      <c r="Z1" s="49" t="inlineStr">
+      <c r="Z1" s="47" t="inlineStr">
         <is>
           <t>Deal_CloseDate</t>
         </is>
       </c>
-      <c r="AA1" s="49" t="inlineStr">
+      <c r="AA1" s="47" t="inlineStr">
         <is>
           <t>Deal_ProposedCmt</t>
         </is>
       </c>
-      <c r="AB1" s="49" t="inlineStr">
+      <c r="AB1" s="47" t="inlineStr">
         <is>
           <t>Deal_DepartmentCode</t>
         </is>
       </c>
-      <c r="AC1" s="49" t="inlineStr">
+      <c r="AC1" s="47" t="inlineStr">
         <is>
           <t>Deal_Department</t>
         </is>
       </c>
-      <c r="AD1" s="49" t="inlineStr">
+      <c r="AD1" s="47" t="inlineStr">
         <is>
           <t>Deal_ExpenseCode</t>
         </is>
       </c>
-      <c r="AE1" s="49" t="inlineStr">
+      <c r="AE1" s="47" t="inlineStr">
         <is>
           <t>HolidayCalendar</t>
         </is>
       </c>
-      <c r="AF1" s="49" t="inlineStr">
+      <c r="AF1" s="47" t="inlineStr">
         <is>
           <t>Deal_PricingOption</t>
         </is>
       </c>
-      <c r="AG1" s="49" t="inlineStr">
+      <c r="AG1" s="47" t="inlineStr">
         <is>
           <t>InitialFractionRate_Round</t>
         </is>
       </c>
-      <c r="AH1" s="49" t="inlineStr">
+      <c r="AH1" s="47" t="inlineStr">
         <is>
           <t>RoundingDecimal_Round</t>
         </is>
       </c>
-      <c r="AI1" s="49" t="inlineStr">
+      <c r="AI1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_RoundingApplicationMethod</t>
         </is>
       </c>
-      <c r="AJ1" s="49" t="inlineStr">
+      <c r="AJ1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_PercentOfRateFormulaUsage</t>
         </is>
       </c>
-      <c r="AK1" s="49" t="inlineStr">
+      <c r="AK1" s="47" t="inlineStr">
         <is>
           <t>NonBusinessDayRule</t>
         </is>
       </c>
-      <c r="AL1" s="49" t="inlineStr">
+      <c r="AL1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_RepricingNonBusinessDayRule</t>
         </is>
       </c>
-      <c r="AM1" s="49" t="inlineStr">
+      <c r="AM1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_BillNoOfDays</t>
         </is>
       </c>
-      <c r="AN1" s="49" t="inlineStr">
+      <c r="AN1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_MatrixChangeAppMthd</t>
         </is>
       </c>
-      <c r="AO1" s="49" t="inlineStr">
+      <c r="AO1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_RateChangeAppMthd</t>
         </is>
       </c>
-      <c r="AP1" s="49" t="inlineStr">
+      <c r="AP1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_InterestDueUponPrincipalPayment</t>
         </is>
       </c>
-      <c r="AQ1" s="49" t="inlineStr">
+      <c r="AQ1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_InterestDueUponRepricing</t>
         </is>
       </c>
-      <c r="AR1" s="49" t="inlineStr">
+      <c r="AR1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_BillBorrower</t>
         </is>
       </c>
-      <c r="AS1" s="49" t="inlineStr">
+      <c r="AS1" s="62" t="inlineStr">
         <is>
           <t>PricingOption_RoundingDecimalPrecision</t>
         </is>
       </c>
-      <c r="AT1" s="49" t="inlineStr">
+      <c r="AT1" s="79" t="inlineStr">
+        <is>
+          <t>PricingOption_ReferenceBanksApply</t>
+        </is>
+      </c>
+      <c r="AU1" s="79" t="inlineStr">
+        <is>
+          <t>PricingOption_IntentNoticeDaysInAdvance</t>
+        </is>
+      </c>
+      <c r="AV1" s="47" t="inlineStr">
         <is>
           <t>PricingOption_InitialFractionRate</t>
         </is>
       </c>
-      <c r="AU1" s="49" t="inlineStr">
+      <c r="AW1" s="47" t="inlineStr">
         <is>
           <t>MinimumPaymentAmount</t>
         </is>
       </c>
-      <c r="AV1" s="49" t="inlineStr">
+      <c r="AX1" s="47" t="inlineStr">
         <is>
           <t>MinimumAmountMultiples</t>
         </is>
       </c>
-      <c r="AW1" s="8" t="inlineStr">
+      <c r="AY1" s="8" t="inlineStr">
         <is>
           <t>MinimumDrawdownAmount</t>
         </is>
       </c>
-      <c r="AX1" s="49" t="inlineStr">
+      <c r="AZ1" s="47" t="inlineStr">
         <is>
           <t>PricingRule_Fee</t>
         </is>
       </c>
-      <c r="AY1" s="49" t="inlineStr">
+      <c r="BA1" s="47" t="inlineStr">
         <is>
           <t>PricingRule_MatrixChangeAppMthd</t>
         </is>
       </c>
-      <c r="AZ1" s="49" t="inlineStr">
+      <c r="BB1" s="47" t="inlineStr">
         <is>
           <t>PricingRule_NonBussDayRule</t>
         </is>
       </c>
-      <c r="BA1" s="49" t="inlineStr">
+      <c r="BC1" s="47" t="inlineStr">
         <is>
           <t>Ratio_Type</t>
         </is>
       </c>
-      <c r="BB1" s="49" t="inlineStr">
+      <c r="BD1" s="47" t="inlineStr">
         <is>
           <t>Ratios_And_Cons_Index</t>
         </is>
       </c>
-      <c r="BC1" s="49" t="inlineStr">
+      <c r="BE1" s="47" t="inlineStr">
         <is>
           <t>Ratios_And_Cons_Description</t>
         </is>
       </c>
-      <c r="BD1" s="49" t="inlineStr">
+      <c r="BF1" s="47" t="inlineStr">
         <is>
           <t>Ratios_And_Cons_StartDate</t>
         </is>
       </c>
-      <c r="BE1" s="49" t="inlineStr">
+      <c r="BG1" s="47" t="inlineStr">
         <is>
           <t>Ratios_And_Cons_RadioButton</t>
         </is>
       </c>
-      <c r="BF1" s="49" t="inlineStr">
+      <c r="BH1" s="47" t="inlineStr">
         <is>
           <t>Financial_Ratio</t>
         </is>
       </c>
-      <c r="BG1" s="49" t="inlineStr">
+      <c r="BI1" s="47" t="inlineStr">
         <is>
           <t>Ratio_StartDate</t>
         </is>
       </c>
-      <c r="BH1" s="49" t="inlineStr">
+      <c r="BJ1" s="47" t="inlineStr">
         <is>
           <t>BankRole_Type</t>
         </is>
       </c>
-      <c r="BI1" s="49" t="inlineStr">
+      <c r="BK1" s="47" t="inlineStr">
         <is>
           <t>Reference_Bank</t>
         </is>
       </c>
-      <c r="BJ1" s="49" t="inlineStr">
+      <c r="BL1" s="47" t="inlineStr">
         <is>
           <t>Bid_Bank</t>
         </is>
       </c>
-      <c r="BK1" s="49" t="inlineStr">
+      <c r="BM1" s="47" t="inlineStr">
         <is>
           <t>SBLC_Issuer</t>
         </is>
       </c>
-      <c r="BL1" s="49" t="inlineStr">
+      <c r="BN1" s="47" t="inlineStr">
         <is>
           <t>Swingline_Bank</t>
         </is>
       </c>
-      <c r="BM1" s="49" t="inlineStr">
+      <c r="BO1" s="47" t="inlineStr">
         <is>
           <t>BA_Issuing_Bank</t>
         </is>
       </c>
-      <c r="BN1" s="49" t="inlineStr">
+      <c r="BP1" s="47" t="inlineStr">
         <is>
           <t>BA_Reference_Bank</t>
         </is>
       </c>
-      <c r="BO1" s="49" t="inlineStr">
+      <c r="BQ1" s="47" t="inlineStr">
         <is>
           <t>BA_Owner_Bank</t>
         </is>
       </c>
-      <c r="BP1" s="49" t="inlineStr">
+      <c r="BR1" s="47" t="inlineStr">
         <is>
           <t>RAC_Reference_Bank</t>
         </is>
       </c>
-      <c r="BQ1" s="49" t="inlineStr">
+      <c r="BS1" s="47" t="inlineStr">
         <is>
           <t>BankRole_Percent</t>
         </is>
       </c>
-      <c r="BR1" s="49" t="inlineStr">
+      <c r="BT1" s="47" t="inlineStr">
         <is>
           <t>BankRole_BankName</t>
         </is>
       </c>
-      <c r="BS1" s="49" t="inlineStr">
+      <c r="BU1" s="47" t="inlineStr">
         <is>
           <t>BankRole_SGAlias</t>
         </is>
       </c>
-      <c r="BT1" s="49" t="inlineStr">
+      <c r="BV1" s="47" t="inlineStr">
         <is>
           <t>BankRole_SGContactName</t>
         </is>
       </c>
-      <c r="BU1" s="49" t="inlineStr">
+      <c r="BW1" s="47" t="inlineStr">
         <is>
           <t>BankRole_SGRIMethod</t>
         </is>
       </c>
-      <c r="BV1" s="49" t="inlineStr">
+      <c r="BX1" s="47" t="inlineStr">
         <is>
           <t>BankRole_SGName</t>
         </is>
       </c>
-      <c r="BW1" s="49" t="inlineStr">
+      <c r="BY1" s="47" t="inlineStr">
         <is>
           <t>BankRole_Portfolio</t>
         </is>
       </c>
-      <c r="BX1" s="49" t="inlineStr">
+      <c r="BZ1" s="47" t="inlineStr">
         <is>
           <t>BankRole_ExpenseCode</t>
         </is>
       </c>
-      <c r="BY1" s="49" t="inlineStr">
+      <c r="CA1" s="47" t="inlineStr">
         <is>
           <t>BankRole_ExpenseCodeDesc</t>
         </is>
       </c>
-      <c r="BZ1" s="49" t="inlineStr">
+      <c r="CB1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_IncomeMethod</t>
         </is>
       </c>
-      <c r="CA1" s="49" t="inlineStr">
+      <c r="CC1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_AmountType</t>
         </is>
       </c>
-      <c r="CB1" s="49" t="inlineStr">
+      <c r="CD1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_Amount</t>
         </is>
       </c>
-      <c r="CC1" s="49" t="inlineStr">
+      <c r="CE1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_EffectiveDate</t>
         </is>
       </c>
-      <c r="CD1" s="49" t="inlineStr">
+      <c r="CF1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_Frequency</t>
         </is>
       </c>
-      <c r="CE1" s="49" t="inlineStr">
+      <c r="CG1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_Customer</t>
         </is>
       </c>
-      <c r="CF1" s="49" t="inlineStr">
+      <c r="CH1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_CustomerLocation</t>
         </is>
       </c>
-      <c r="CG1" s="49" t="inlineStr">
+      <c r="CI1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_ExpenseCode</t>
         </is>
       </c>
-      <c r="CH1" s="49" t="inlineStr">
+      <c r="CJ1" s="47" t="inlineStr">
         <is>
           <t>AdminFee_PercentOfFee</t>
         </is>
       </c>
-      <c r="CI1" s="49" t="inlineStr">
+      <c r="CK1" s="47" t="inlineStr">
         <is>
           <t>UpfrontFee_Category</t>
         </is>
       </c>
-      <c r="CJ1" s="49" t="inlineStr">
+      <c r="CL1" s="47" t="inlineStr">
         <is>
           <t>UpfrontFee_Type</t>
         </is>
       </c>
-      <c r="CK1" s="49" t="inlineStr">
+      <c r="CM1" s="47" t="inlineStr">
         <is>
           <t>UpfrontFee_RateBasis</t>
         </is>
       </c>
-      <c r="CL1" s="49" t="inlineStr">
+      <c r="CN1" s="47" t="inlineStr">
         <is>
           <t>UpfrontFee_Amount</t>
         </is>
       </c>
-      <c r="CM1" s="49" t="inlineStr">
+      <c r="CO1" s="47" t="inlineStr">
         <is>
           <t>UpfrontFeePayment_Comment</t>
         </is>
       </c>
-      <c r="CN1" s="49" t="inlineStr">
+      <c r="CP1" s="47" t="inlineStr">
         <is>
           <t>EstablishmentFee_EffectiveDate</t>
         </is>
       </c>
-      <c r="CO1" s="49" t="inlineStr">
+      <c r="CQ1" s="47" t="inlineStr">
         <is>
           <t>Deal_SalesGroup</t>
         </is>
       </c>
-      <c r="CP1" s="49" t="inlineStr">
+      <c r="CR1" s="47" t="inlineStr">
         <is>
           <t>Borrower_PreferredRIMthd1</t>
         </is>
       </c>
-      <c r="CQ1" s="49" t="inlineStr">
+      <c r="CS1" s="47" t="inlineStr">
         <is>
           <t>Borrower_RemittanceDescription</t>
         </is>
@@ -2008,17 +2088,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_33103</t>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_32153</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>33105</t>
+          <t>32153</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CLASS A DEBTHOLDERS44103</t>
+          <t>CLASS A DEBTHOLDERS44128</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2161,60 +2241,70 @@
           <t>ON</t>
         </is>
       </c>
-      <c r="AS2" s="25" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AT2" s="25" t="inlineStr">
+      <c r="AS2" s="66" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AT2" s="8" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="AU2" s="80" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AV2" s="25" t="inlineStr">
         <is>
           <t>1/8</t>
         </is>
       </c>
-      <c r="AV2" s="25" t="inlineStr">
+      <c r="AX2" s="25" t="inlineStr">
         <is>
           <t>0.01</t>
         </is>
       </c>
-      <c r="AW2" s="25" t="inlineStr">
+      <c r="AY2" s="25" t="inlineStr">
         <is>
           <t>500000</t>
         </is>
       </c>
-      <c r="AX2" s="25" t="inlineStr">
+      <c r="AZ2" s="25" t="inlineStr">
         <is>
           <t>Commitment Fee</t>
         </is>
       </c>
-      <c r="AY2" s="8" t="inlineStr">
+      <c r="BA2" s="8" t="inlineStr">
         <is>
           <t>Start of current cycle</t>
         </is>
       </c>
-      <c r="AZ2" s="8" t="inlineStr">
+      <c r="BB2" s="8" t="inlineStr">
         <is>
           <t>Next Business Day</t>
         </is>
       </c>
-      <c r="BB2" s="25" t="inlineStr">
+      <c r="BD2" s="25" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="BC2" s="8" t="inlineStr">
+      <c r="BE2" s="8" t="inlineStr">
         <is>
           <t>average unfunded committed account &gt;40%</t>
         </is>
       </c>
-      <c r="BD2" s="58" t="n">
+      <c r="BF2" s="56" t="n">
         <v>43754</v>
       </c>
-      <c r="BE2" t="inlineStr">
+      <c r="BG2" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="CO2" t="inlineStr">
+      <c r="CQ2" t="inlineStr">
         <is>
           <t>Sales Group 1</t>
         </is>
@@ -2235,7 +2325,7 @@
   <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2497,12 +2587,12 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_33103</t>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_32153</t>
         </is>
       </c>
       <c r="E2" s="8" t="inlineStr">
         <is>
-          <t>CLASS A DEBTHOLDERS44103</t>
+          <t>CLASS A DEBTHOLDERS44128</t>
         </is>
       </c>
       <c r="F2" s="25" t="inlineStr">
@@ -2532,12 +2622,12 @@
       </c>
       <c r="K2" s="28" t="inlineStr">
         <is>
-          <t>19-Feb-2021</t>
+          <t>19-Feb-2025</t>
         </is>
       </c>
       <c r="L2" s="28" t="inlineStr">
         <is>
-          <t>19-Feb-2021</t>
+          <t>19-Feb-2025</t>
         </is>
       </c>
       <c r="M2" s="8" t="inlineStr">
@@ -2903,7 +2993,7 @@
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
-          <t>CLASS A DEBTHOLDERS44103</t>
+          <t>CLASS A DEBTHOLDERS44128</t>
         </is>
       </c>
       <c r="D2" s="8" t="inlineStr">
@@ -3038,7 +3128,7 @@
       <c r="AS2" s="43" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="24">
-      <c r="Z3" s="57" t="n"/>
+      <c r="Z3" s="55" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3053,7 +3143,7 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -3166,22 +3256,22 @@
           <t>Lender2_ShortName</t>
         </is>
       </c>
-      <c r="T1" s="50" t="inlineStr">
+      <c r="T1" s="48" t="inlineStr">
         <is>
           <t>Lender_RemittanceDescription</t>
         </is>
       </c>
-      <c r="U1" s="50" t="inlineStr">
+      <c r="U1" s="48" t="inlineStr">
         <is>
           <t>Lender2_RemittanceDescription</t>
         </is>
       </c>
-      <c r="V1" s="50" t="inlineStr">
+      <c r="V1" s="48" t="inlineStr">
         <is>
           <t>Lender_RemittanceInstruction</t>
         </is>
       </c>
-      <c r="W1" s="50" t="inlineStr">
+      <c r="W1" s="48" t="inlineStr">
         <is>
           <t>Lender2_RemittanceInstruction</t>
         </is>
@@ -3255,7 +3345,7 @@
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_33103</t>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_32153</t>
         </is>
       </c>
       <c r="D2" s="25" t="inlineStr">
@@ -3265,7 +3355,7 @@
       </c>
       <c r="E2" s="8" t="inlineStr">
         <is>
-          <t>CLASS A DEBTHOLDERS44103</t>
+          <t>CLASS A DEBTHOLDERS44128</t>
         </is>
       </c>
       <c r="F2" s="28" t="inlineStr">
@@ -3293,30 +3383,30 @@
           <t>14-Jan-2020</t>
         </is>
       </c>
-      <c r="K2" s="47" t="n"/>
-      <c r="L2" s="47" t="n"/>
-      <c r="M2" s="47" t="n"/>
+      <c r="K2" s="46" t="n"/>
+      <c r="L2" s="46" t="n"/>
+      <c r="M2" s="46" t="n"/>
       <c r="N2" s="44" t="n"/>
       <c r="O2" s="44" t="n"/>
-      <c r="P2" s="47" t="n"/>
+      <c r="P2" s="46" t="n"/>
       <c r="Q2" s="44" t="n"/>
-      <c r="R2" s="52" t="n"/>
-      <c r="S2" s="52" t="n"/>
+      <c r="R2" s="50" t="n"/>
+      <c r="S2" s="50" t="n"/>
       <c r="T2" s="44" t="n"/>
       <c r="U2" s="44" t="n"/>
       <c r="V2" s="44" t="n"/>
       <c r="W2" s="44" t="n"/>
       <c r="X2" s="44" t="n"/>
       <c r="Y2" s="44" t="n"/>
-      <c r="Z2" s="46" t="n"/>
+      <c r="Z2" s="45" t="n"/>
       <c r="AA2" s="44" t="n"/>
-      <c r="AB2" s="53" t="n"/>
-      <c r="AC2" s="47" t="n"/>
-      <c r="AD2" s="47" t="n"/>
-      <c r="AE2" s="54" t="n"/>
-      <c r="AF2" s="54" t="n"/>
-      <c r="AG2" s="54" t="n"/>
-      <c r="AH2" s="47" t="n"/>
+      <c r="AB2" s="51" t="n"/>
+      <c r="AC2" s="46" t="n"/>
+      <c r="AD2" s="46" t="n"/>
+      <c r="AE2" s="52" t="n"/>
+      <c r="AF2" s="52" t="n"/>
+      <c r="AG2" s="52" t="n"/>
+      <c r="AH2" s="46" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3332,7 +3422,7 @@
   </sheetPr>
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -3368,116 +3458,116 @@
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="51" t="inlineStr">
+      <c r="C1" s="49" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="51" t="inlineStr">
+      <c r="D1" s="49" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="E1" s="49" t="inlineStr">
+      <c r="E1" s="47" t="inlineStr">
         <is>
           <t>Primary_Lender</t>
         </is>
       </c>
-      <c r="F1" s="49" t="inlineStr">
+      <c r="F1" s="47" t="inlineStr">
         <is>
           <t>Primary_LenderLoc1</t>
         </is>
       </c>
-      <c r="G1" s="49" t="inlineStr">
+      <c r="G1" s="47" t="inlineStr">
         <is>
           <t>Primary_RiskBook</t>
         </is>
       </c>
-      <c r="H1" s="49" t="inlineStr">
+      <c r="H1" s="47" t="inlineStr">
         <is>
           <t>Primaries_TransactionType</t>
         </is>
       </c>
-      <c r="I1" s="49" t="inlineStr">
+      <c r="I1" s="47" t="inlineStr">
         <is>
           <t>Primary_PctOfDeal</t>
         </is>
       </c>
-      <c r="J1" s="49" t="inlineStr">
+      <c r="J1" s="47" t="inlineStr">
         <is>
           <t>Primary_BuySellPrice</t>
         </is>
       </c>
-      <c r="K1" s="49" t="inlineStr">
+      <c r="K1" s="47" t="inlineStr">
         <is>
           <t>Primary_Contact</t>
         </is>
       </c>
-      <c r="L1" s="49" t="inlineStr">
+      <c r="L1" s="47" t="inlineStr">
         <is>
           <t>Primary_ServicingGroupMember</t>
         </is>
       </c>
-      <c r="M1" s="49" t="inlineStr">
+      <c r="M1" s="47" t="inlineStr">
         <is>
           <t>Primary_SGAlias</t>
         </is>
       </c>
-      <c r="N1" s="49" t="inlineStr">
+      <c r="N1" s="47" t="inlineStr">
         <is>
           <t>Primary_CircledDate</t>
         </is>
       </c>
-      <c r="O1" s="49" t="inlineStr">
+      <c r="O1" s="47" t="inlineStr">
         <is>
           <t>Primary_ExpiryDate</t>
         </is>
       </c>
-      <c r="P1" s="49" t="inlineStr">
+      <c r="P1" s="47" t="inlineStr">
         <is>
           <t>ExpenseCode_Description</t>
         </is>
       </c>
-      <c r="Q1" s="49" t="inlineStr">
+      <c r="Q1" s="47" t="inlineStr">
         <is>
           <t>Primary_Portfolio</t>
         </is>
       </c>
-      <c r="R1" s="49" t="inlineStr">
+      <c r="R1" s="47" t="inlineStr">
         <is>
           <t>Primary_PortfolioBranch</t>
         </is>
       </c>
-      <c r="S1" s="49" t="inlineStr">
+      <c r="S1" s="47" t="inlineStr">
         <is>
           <t>ApproveDate</t>
         </is>
       </c>
-      <c r="T1" s="49" t="inlineStr">
+      <c r="T1" s="47" t="inlineStr">
         <is>
           <t>CloseDate</t>
         </is>
       </c>
-      <c r="U1" s="49" t="inlineStr">
+      <c r="U1" s="47" t="inlineStr">
         <is>
           <t>Lender_Hostbank</t>
         </is>
       </c>
-      <c r="V1" s="49" t="inlineStr">
+      <c r="V1" s="47" t="inlineStr">
         <is>
           <t>Orig_Primary_ExpectedCloseDate</t>
         </is>
       </c>
-      <c r="X1" s="49" t="n"/>
-      <c r="Y1" s="49" t="n"/>
-      <c r="Z1" s="49" t="n"/>
-      <c r="AA1" s="49" t="n"/>
-      <c r="AB1" s="49" t="n"/>
-      <c r="AC1" s="49" t="n"/>
-      <c r="AD1" s="49" t="n"/>
+      <c r="X1" s="47" t="n"/>
+      <c r="Y1" s="47" t="n"/>
+      <c r="Z1" s="47" t="n"/>
+      <c r="AA1" s="47" t="n"/>
+      <c r="AB1" s="47" t="n"/>
+      <c r="AC1" s="47" t="n"/>
+      <c r="AD1" s="47" t="n"/>
     </row>
     <row r="2" ht="15" customHeight="1" s="24">
-      <c r="A2" s="55" t="inlineStr">
+      <c r="A2" s="53" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3489,40 +3579,40 @@
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_33103</t>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_32153</t>
         </is>
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>CLASS A DEBTHOLDERS44103</t>
-        </is>
-      </c>
-      <c r="E2" s="59" t="inlineStr">
+          <t>CLASS A DEBTHOLDERS44128</t>
+        </is>
+      </c>
+      <c r="E2" s="57" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="F2" s="59" t="inlineStr">
+      <c r="F2" s="57" t="inlineStr">
         <is>
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="G2" s="56" t="inlineStr">
+      <c r="G2" s="54" t="inlineStr">
         <is>
           <t>DM_AGY</t>
         </is>
       </c>
-      <c r="H2" s="59" t="inlineStr">
+      <c r="H2" s="57" t="inlineStr">
         <is>
           <t>Origination</t>
         </is>
       </c>
-      <c r="I2" s="59" t="inlineStr">
+      <c r="I2" s="57" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="J2" s="56" t="inlineStr">
+      <c r="J2" s="54" t="inlineStr">
         <is>
           <t>100</t>
         </is>
@@ -3532,7 +3622,7 @@
           <t>NON AGENCY</t>
         </is>
       </c>
-      <c r="L2" s="63" t="inlineStr">
+      <c r="L2" s="61" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3542,23 +3632,23 @@
           <t>NON AGENCY</t>
         </is>
       </c>
-      <c r="N2" s="60" t="inlineStr">
+      <c r="N2" s="58" t="inlineStr">
         <is>
           <t>24-Nov-2015</t>
         </is>
       </c>
-      <c r="O2" s="62" t="inlineStr">
+      <c r="O2" s="60" t="inlineStr">
         <is>
           <t>30-Dec-2022</t>
         </is>
       </c>
       <c r="P2" s="8" t="n"/>
-      <c r="Q2" s="61" t="inlineStr">
+      <c r="Q2" s="59" t="inlineStr">
         <is>
           <t>Hold for Investment - Australia</t>
         </is>
       </c>
-      <c r="R2" s="61" t="inlineStr">
+      <c r="R2" s="59" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
@@ -3600,208 +3690,683 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AD2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="10.140625" bestFit="1" customWidth="1" style="24" min="2" max="2"/>
-    <col width="11.42578125" bestFit="1" customWidth="1" style="24" min="3" max="3"/>
-    <col width="14" bestFit="1" customWidth="1" style="24" min="4" max="4"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="24" min="2" max="2"/>
+    <col width="42.42578125" bestFit="1" customWidth="1" style="24" min="3" max="3"/>
+    <col width="28.85546875" bestFit="1" customWidth="1" style="24" min="4" max="4"/>
     <col width="11" bestFit="1" customWidth="1" style="24" min="5" max="5"/>
-    <col width="15.85546875" bestFit="1" customWidth="1" style="24" min="6" max="6"/>
+    <col width="22.5703125" bestFit="1" customWidth="1" style="24" min="6" max="6"/>
     <col width="31.5703125" bestFit="1" customWidth="1" style="24" min="7" max="7"/>
-    <col width="30.85546875" bestFit="1" customWidth="1" style="24" min="8" max="8"/>
-    <col width="7.42578125" bestFit="1" customWidth="1" style="24" min="9" max="9"/>
-    <col width="17.5703125" bestFit="1" customWidth="1" style="24" min="19" max="19"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="24" min="8" max="8"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" style="24" min="9" max="9"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="24" min="10" max="10"/>
+    <col width="29.42578125" bestFit="1" customWidth="1" style="24" min="11" max="11"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" style="24" min="12" max="12"/>
+    <col width="23.85546875" bestFit="1" customWidth="1" style="24" min="13" max="13"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="24" min="14" max="14"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="24" min="15" max="15"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="24" min="16" max="16"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="24" min="17" max="17"/>
+    <col width="23.85546875" bestFit="1" customWidth="1" style="24" min="19" max="19"/>
+    <col width="24.28515625" bestFit="1" customWidth="1" style="24" min="20" max="20"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="24" min="30" max="30"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customFormat="1" customHeight="1" s="49">
-      <c r="A1" s="49" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="62" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="49" t="inlineStr">
+      <c r="B1" s="62" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="50" t="inlineStr">
+      <c r="C1" s="63" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="50" t="inlineStr">
+      <c r="D1" s="63" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="E1" s="50" t="inlineStr">
+      <c r="E1" s="63" t="inlineStr">
         <is>
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="F1" s="50" t="inlineStr">
+      <c r="F1" s="63" t="inlineStr">
         <is>
           <t>Borrower_Name</t>
         </is>
       </c>
-      <c r="G1" s="50" t="inlineStr">
-        <is>
-          <t>Borrower_RemittanceDescription</t>
-        </is>
-      </c>
-      <c r="H1" s="50" t="inlineStr">
-        <is>
-          <t>Borrower_RemittanceInstruction</t>
-        </is>
-      </c>
-      <c r="I1" s="50" t="inlineStr">
+      <c r="G1" s="62" t="inlineStr">
+        <is>
+          <t>Outstanding_Type</t>
+        </is>
+      </c>
+      <c r="H1" s="62" t="inlineStr">
+        <is>
+          <t>Pricing_Option</t>
+        </is>
+      </c>
+      <c r="I1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_RequestedAmount</t>
+        </is>
+      </c>
+      <c r="J1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_EffectiveDate</t>
+        </is>
+      </c>
+      <c r="K1" s="64" t="inlineStr">
+        <is>
+          <t>Loan_MaturityDate</t>
+        </is>
+      </c>
+      <c r="L1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_RepricingFrequency</t>
+        </is>
+      </c>
+      <c r="M1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_IntCycleFrequency</t>
+        </is>
+      </c>
+      <c r="N1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_Accrue</t>
+        </is>
+      </c>
+      <c r="O1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_RepricingDate</t>
+        </is>
+      </c>
+      <c r="P1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_AccrualEndDate</t>
+        </is>
+      </c>
+      <c r="Q1" s="64" t="inlineStr">
+        <is>
+          <t>Remittance_Description</t>
+        </is>
+      </c>
+      <c r="R1" s="64" t="inlineStr">
+        <is>
+          <t>Remittance_Instruction</t>
+        </is>
+      </c>
+      <c r="S1" s="64" t="inlineStr">
+        <is>
+          <t>AcceptRate_FromPricing</t>
+        </is>
+      </c>
+      <c r="T1" s="64" t="inlineStr">
+        <is>
+          <t>RateSetting_NoticeStatus</t>
+        </is>
+      </c>
+      <c r="U1" s="63" t="inlineStr">
         <is>
           <t>Lender</t>
         </is>
       </c>
-      <c r="J1" s="50" t="inlineStr">
+      <c r="V1" s="63" t="inlineStr">
         <is>
           <t>Lender2</t>
         </is>
       </c>
-      <c r="K1" s="50" t="inlineStr">
+      <c r="W1" s="63" t="inlineStr">
         <is>
           <t>Lender_RemittanceDescription</t>
         </is>
       </c>
-      <c r="L1" s="50" t="inlineStr">
+      <c r="X1" s="63" t="inlineStr">
         <is>
           <t>Lender2_RemittanceDescription</t>
         </is>
       </c>
-      <c r="M1" s="50" t="inlineStr">
+      <c r="Y1" s="63" t="inlineStr">
         <is>
           <t>Lender_RemittanceInstruction</t>
         </is>
       </c>
-      <c r="N1" s="50" t="inlineStr">
+      <c r="Z1" s="63" t="inlineStr">
         <is>
           <t>Lender2_RemittanceInstruction</t>
         </is>
       </c>
-      <c r="O1" s="50" t="inlineStr">
-        <is>
-          <t>Pricing_Option</t>
-        </is>
-      </c>
-      <c r="P1" s="50" t="inlineStr">
+      <c r="AA1" s="63" t="inlineStr">
         <is>
           <t>HostBank_LenderShare</t>
         </is>
       </c>
-      <c r="Q1" s="50" t="inlineStr">
+      <c r="AB1" s="63" t="inlineStr">
         <is>
           <t>Lender1_Share</t>
         </is>
       </c>
-      <c r="R1" s="50" t="inlineStr">
+      <c r="AC1" s="63" t="inlineStr">
         <is>
           <t>Lender2_Share</t>
         </is>
       </c>
-      <c r="S1" s="49" t="inlineStr">
-        <is>
-          <t>Outstanding_Type</t>
-        </is>
-      </c>
-      <c r="T1" s="49" t="inlineStr">
+      <c r="AD1" s="62" t="inlineStr">
         <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="U1" s="49" t="inlineStr">
-        <is>
-          <t>Loan_RequestedAmount</t>
-        </is>
-      </c>
-      <c r="V1" s="49" t="inlineStr">
+      <c r="AE1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_BorrowerBaseRate</t>
+        </is>
+      </c>
+      <c r="AF1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_FacilitySpread</t>
+        </is>
+      </c>
+      <c r="AG1" s="62" t="inlineStr">
+        <is>
+          <t>Loan_OverrideSpread</t>
+        </is>
+      </c>
+      <c r="AH1" s="62" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="24">
+      <c r="A2" s="59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="59" t="inlineStr">
+        <is>
+          <t>Deal_PIM_Future_BILAT</t>
+        </is>
+      </c>
+      <c r="C2" s="59" t="inlineStr">
+        <is>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_32153</t>
+        </is>
+      </c>
+      <c r="D2" s="44" t="inlineStr">
+        <is>
+          <t>CLASS A DEBTHOLDERS44128</t>
+        </is>
+      </c>
+      <c r="E2" s="59" t="inlineStr">
+        <is>
+          <t>60001970</t>
+        </is>
+      </c>
+      <c r="F2" s="59" t="inlineStr">
+        <is>
+          <t>NEW JB TRUST 1915659</t>
+        </is>
+      </c>
+      <c r="G2" s="59" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="H2" s="59" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="I2" s="65" t="inlineStr">
+        <is>
+          <t>191,569,254.72</t>
+        </is>
+      </c>
+      <c r="J2" s="66" t="inlineStr">
+        <is>
+          <t>19-Dec-2019</t>
+        </is>
+      </c>
+      <c r="K2" s="60" t="inlineStr">
+        <is>
+          <t>19-Feb-2025</t>
+        </is>
+      </c>
+      <c r="L2" s="59" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+      <c r="M2" s="67" t="n"/>
+      <c r="N2" s="59" t="inlineStr">
+        <is>
+          <t>to the adjusted due date</t>
+        </is>
+      </c>
+      <c r="O2" s="66" t="inlineStr">
+        <is>
+          <t>21-Jan-2020</t>
+        </is>
+      </c>
+      <c r="P2" s="66" t="n"/>
+      <c r="Q2" s="59" t="n"/>
+      <c r="R2" s="59" t="n"/>
+      <c r="S2" s="59" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="T2" s="59" t="inlineStr">
+        <is>
+          <t>Awaiting release</t>
+        </is>
+      </c>
+      <c r="U2" s="68" t="n"/>
+      <c r="V2" s="68" t="n"/>
+      <c r="W2" s="69" t="n"/>
+      <c r="X2" s="69" t="n"/>
+      <c r="Y2" s="69" t="n"/>
+      <c r="Z2" s="69" t="n"/>
+      <c r="AA2" s="69" t="n"/>
+      <c r="AB2" s="69" t="n"/>
+      <c r="AC2" s="69" t="n"/>
+      <c r="AD2" s="69" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AE2" s="69" t="n"/>
+      <c r="AF2" s="69" t="n"/>
+      <c r="AG2" s="69" t="n"/>
+      <c r="AH2" s="70" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BL4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" ht="12.75" customFormat="1" customHeight="1" s="77">
+      <c r="A1" s="71" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="71" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="72" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="72" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="72" t="inlineStr">
+        <is>
+          <t>Loan_Alias</t>
+        </is>
+      </c>
+      <c r="F1" s="71" t="inlineStr">
+        <is>
+          <t>SubAdd_Days</t>
+        </is>
+      </c>
+      <c r="G1" s="73" t="inlineStr">
+        <is>
+          <t>Notice_Type</t>
+        </is>
+      </c>
+      <c r="H1" s="72" t="inlineStr">
+        <is>
+          <t>Notice_Customer_LegalName</t>
+        </is>
+      </c>
+      <c r="I1" s="72" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="J1" s="71" t="inlineStr">
+        <is>
+          <t>NoticeGroup_UserID</t>
+        </is>
+      </c>
+      <c r="K1" s="72" t="inlineStr">
+        <is>
+          <t>Notice_Identifier</t>
+        </is>
+      </c>
+      <c r="L1" s="72" t="inlineStr">
+        <is>
+          <t>Correlation_ID</t>
+        </is>
+      </c>
+      <c r="M1" s="72" t="inlineStr">
+        <is>
+          <t>Thru_Date</t>
+        </is>
+      </c>
+      <c r="N1" s="72" t="inlineStr">
+        <is>
+          <t>From_Date</t>
+        </is>
+      </c>
+      <c r="O1" s="71" t="inlineStr">
+        <is>
+          <t>Search_By</t>
+        </is>
+      </c>
+      <c r="P1" s="72" t="inlineStr">
+        <is>
+          <t>Notice_Method</t>
+        </is>
+      </c>
+      <c r="Q1" s="72" t="inlineStr">
+        <is>
+          <t>BEO_StartDate</t>
+        </is>
+      </c>
+      <c r="R1" s="72" t="inlineStr">
+        <is>
+          <t>BEO_EndDate</t>
+        </is>
+      </c>
+      <c r="S1" s="71" t="inlineStr">
+        <is>
+          <t>Customer_IdentifiedBy</t>
+        </is>
+      </c>
+      <c r="T1" s="71" t="inlineStr">
+        <is>
+          <t>Zero_TempPath</t>
+        </is>
+      </c>
+      <c r="U1" s="71" t="inlineStr">
+        <is>
+          <t>InputFilePath</t>
+        </is>
+      </c>
+      <c r="V1" s="71" t="inlineStr">
+        <is>
+          <t>XML_File</t>
+        </is>
+      </c>
+      <c r="W1" s="71" t="inlineStr">
+        <is>
+          <t>Temp_File</t>
+        </is>
+      </c>
+      <c r="X1" s="71" t="inlineStr">
+        <is>
+          <t>InputJson</t>
+        </is>
+      </c>
+      <c r="Y1" s="71" t="inlineStr">
+        <is>
+          <t>ExpectedJson</t>
+        </is>
+      </c>
+      <c r="Z1" s="71" t="inlineStr">
+        <is>
+          <t>OutputFilePath</t>
+        </is>
+      </c>
+      <c r="AA1" s="71" t="inlineStr">
+        <is>
+          <t>Field_Name</t>
+        </is>
+      </c>
+      <c r="AB1" s="71" t="inlineStr">
+        <is>
+          <t>OutputAPIResponse</t>
+        </is>
+      </c>
+      <c r="AC1" s="74" t="inlineStr">
+        <is>
+          <t>messageId</t>
+        </is>
+      </c>
+      <c r="AD1" s="74" t="inlineStr">
+        <is>
+          <t>CallBack_Status</t>
+        </is>
+      </c>
+      <c r="AE1" s="74" t="inlineStr">
+        <is>
+          <t>CallBack_Status2</t>
+        </is>
+      </c>
+      <c r="AF1" s="75" t="inlineStr">
+        <is>
+          <t>errorMessage</t>
+        </is>
+      </c>
+      <c r="AG1" s="74" t="inlineStr">
+        <is>
+          <t>errorMessage_2</t>
+        </is>
+      </c>
+      <c r="AH1" s="71" t="inlineStr">
+        <is>
+          <t>Notice_Status</t>
+        </is>
+      </c>
+      <c r="AI1" s="71" t="inlineStr">
+        <is>
+          <t>WIP_ExceptionQueueDescription</t>
+        </is>
+      </c>
+      <c r="AJ1" s="76" t="inlineStr">
+        <is>
+          <t>XML_NoticeType</t>
+        </is>
+      </c>
+      <c r="AK1" s="76" t="inlineStr">
+        <is>
+          <t>Loan_PricingOption</t>
+        </is>
+      </c>
+      <c r="AL1" s="76" t="inlineStr">
+        <is>
+          <t>OngoingFee_Type</t>
+        </is>
+      </c>
+      <c r="AM1" s="71" t="inlineStr">
+        <is>
+          <t>Balance_Amount</t>
+        </is>
+      </c>
+      <c r="AN1" s="71" t="inlineStr">
+        <is>
+          <t>Rate_Basis</t>
+        </is>
+      </c>
+      <c r="AO1" s="71" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="AP1" s="72" t="inlineStr">
+        <is>
+          <t>Loan_BaseRate</t>
+        </is>
+      </c>
+      <c r="AQ1" s="72" t="inlineStr">
+        <is>
+          <t>Loan_Spread</t>
+        </is>
+      </c>
+      <c r="AR1" s="72" t="inlineStr">
+        <is>
+          <t>Notice_AllInRate</t>
+        </is>
+      </c>
+      <c r="AS1" s="72" t="inlineStr">
+        <is>
+          <t>Notice_Amount</t>
+        </is>
+      </c>
+      <c r="AT1" s="72" t="inlineStr">
         <is>
           <t>Loan_EffectiveDate</t>
         </is>
       </c>
-      <c r="W1" s="51" t="inlineStr">
+      <c r="AU1" s="72" t="inlineStr">
         <is>
           <t>Loan_MaturityDate</t>
         </is>
       </c>
-      <c r="X1" s="49" t="inlineStr">
-        <is>
-          <t>Loan_IntCycleFrequency</t>
-        </is>
-      </c>
-      <c r="Y1" s="49" t="inlineStr">
-        <is>
-          <t>Loan_BorrowerBaseRate</t>
-        </is>
-      </c>
-      <c r="Z1" s="49" t="inlineStr">
-        <is>
-          <t>Loan_FacilitySpread</t>
-        </is>
-      </c>
-      <c r="AA1" s="49" t="inlineStr">
-        <is>
-          <t>Loan_OverrideSpread</t>
-        </is>
-      </c>
-      <c r="AB1" s="49" t="inlineStr">
-        <is>
-          <t>Loan_RepricingFrequency</t>
+      <c r="AV1" s="72" t="inlineStr">
+        <is>
+          <t>Loan_GlobalOriginal</t>
+        </is>
+      </c>
+      <c r="AW1" s="72" t="inlineStr">
+        <is>
+          <t>Loan_RateSetting_DueDate</t>
+        </is>
+      </c>
+      <c r="AX1" s="72" t="inlineStr">
+        <is>
+          <t>Loan_RepricingDate</t>
+        </is>
+      </c>
+      <c r="AY1" s="72" t="inlineStr">
+        <is>
+          <t>EffectiveDate_PrincipalPayment</t>
+        </is>
+      </c>
+      <c r="AZ1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_PrincipalPayment</t>
+        </is>
+      </c>
+      <c r="BA1" s="72" t="inlineStr">
+        <is>
+          <t>EffectiveDate_InterestPayment</t>
+        </is>
+      </c>
+      <c r="BB1" s="72" t="inlineStr">
+        <is>
+          <t>ProjectedCycleDue_InterestPayment</t>
+        </is>
+      </c>
+      <c r="BC1" s="71" t="inlineStr">
+        <is>
+          <t>StartDate_Principal</t>
+        </is>
+      </c>
+      <c r="BD1" s="71" t="inlineStr">
+        <is>
+          <t>EndDate_Principal</t>
+        </is>
+      </c>
+      <c r="BE1" s="71" t="inlineStr">
+        <is>
+          <t>Days_Principal</t>
+        </is>
+      </c>
+      <c r="BF1" s="71" t="inlineStr">
+        <is>
+          <t>Principal_Amount</t>
+        </is>
+      </c>
+      <c r="BG1" s="71" t="inlineStr">
+        <is>
+          <t>StartDate_Interest</t>
+        </is>
+      </c>
+      <c r="BH1" s="71" t="inlineStr">
+        <is>
+          <t>EndDate_Interest</t>
+        </is>
+      </c>
+      <c r="BI1" s="71" t="inlineStr">
+        <is>
+          <t>Days_Interest</t>
+        </is>
+      </c>
+      <c r="BJ1" s="71" t="inlineStr">
+        <is>
+          <t>Interest_Amount</t>
+        </is>
+      </c>
+      <c r="BK1" s="71" t="inlineStr">
+        <is>
+          <t>Fee_Type</t>
+        </is>
+      </c>
+      <c r="BL1" s="72" t="inlineStr">
+        <is>
+          <t>Currency</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customFormat="1" customHeight="1" s="40">
-      <c r="A2" s="44" t="inlineStr">
+    <row r="2">
+      <c r="A2" s="78" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="44" t="n"/>
-      <c r="C2" s="44" t="n"/>
-      <c r="D2" s="44" t="inlineStr">
-        <is>
-          <t>CLASS A DEBTHOLDERS44103</t>
-        </is>
-      </c>
-      <c r="E2" s="44" t="n"/>
-      <c r="F2" s="8" t="n"/>
-      <c r="G2" s="44" t="n"/>
-      <c r="H2" s="44" t="n"/>
-      <c r="I2" s="45" t="n"/>
-      <c r="J2" s="45" t="n"/>
-      <c r="K2" s="44" t="n"/>
-      <c r="L2" s="44" t="n"/>
-      <c r="M2" s="44" t="n"/>
-      <c r="N2" s="44" t="n"/>
-      <c r="O2" s="44" t="n"/>
-      <c r="P2" s="46" t="n"/>
-      <c r="Q2" s="44" t="n"/>
-      <c r="R2" s="44" t="n"/>
-      <c r="S2" s="44" t="n"/>
-      <c r="T2" s="44" t="n"/>
-      <c r="U2" s="39" t="n"/>
-      <c r="V2" s="47" t="n"/>
-      <c r="W2" s="48" t="inlineStr">
-        <is>
-          <t>19-Feb-2021</t>
-        </is>
-      </c>
-      <c r="X2" s="44" t="n"/>
-      <c r="Y2" s="44" t="n"/>
-      <c r="Z2" s="44" t="n"/>
-      <c r="AA2" s="44" t="n"/>
-      <c r="AB2" s="44" t="n"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>60001970</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="78" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>60001970</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="78" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>60001970</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GDE-9316 -replace None args with data from excel
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E168436-ABBF-4742-BB07-C692413461FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCF2102-AAE1-45B3-8A14-38B1C9B07884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" tabRatio="877" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="488">
   <si>
     <t>rowid</t>
   </si>
@@ -1485,6 +1485,12 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>PricingOption_FeeOnLenderShareFunding</t>
+  </si>
+  <si>
+    <t>PricingOption_IntentNoticeTime</t>
   </si>
 </sst>
 </file>
@@ -2727,10 +2733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:CS2"/>
+  <dimension ref="A1:CU2"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT2" sqref="AT2"/>
+    <sheetView topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2766,31 +2772,32 @@
     <col min="36" max="36" width="41.7109375" style="24" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="43.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="26.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="36" style="24" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="34.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="46.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="39.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="26.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="40.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="40.42578125" style="24" customWidth="1"/>
-    <col min="48" max="48" width="31.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="24.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="25" style="24" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="25" style="24" customWidth="1"/>
-    <col min="52" max="52" width="16.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="34.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="28.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="11.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="38.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="28.28515625" style="24" customWidth="1"/>
-    <col min="59" max="59" width="23.7109375" style="24" customWidth="1"/>
-    <col min="60" max="61" width="15.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="16.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="43.28515625" style="24" customWidth="1"/>
+    <col min="40" max="40" width="26.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="36" style="24" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="34.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="46.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="39.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="40.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="40.42578125" style="24" customWidth="1"/>
+    <col min="50" max="50" width="31.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="24.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="25" style="24" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="25" style="24" customWidth="1"/>
+    <col min="54" max="54" width="16.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="34.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="28.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="23.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="38.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="28.28515625" style="24" customWidth="1"/>
+    <col min="61" max="61" width="23.7109375" style="24" customWidth="1"/>
+    <col min="62" max="63" width="15.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.85546875" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" s="47" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" s="47" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2906,184 +2913,190 @@
         <v>148</v>
       </c>
       <c r="AM1" s="47" t="s">
+        <v>486</v>
+      </c>
+      <c r="AN1" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="AN1" s="47" t="s">
+      <c r="AO1" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="AO1" s="47" t="s">
+      <c r="AP1" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="AP1" s="47" t="s">
+      <c r="AQ1" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="AQ1" s="47" t="s">
+      <c r="AR1" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="AR1" s="47" t="s">
+      <c r="AS1" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="AS1" s="62" t="s">
+      <c r="AT1" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="AT1" s="79" t="s">
+      <c r="AU1" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="AU1" s="79" t="s">
+      <c r="AV1" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="AV1" s="47" t="s">
+      <c r="AW1" s="79" t="s">
+        <v>487</v>
+      </c>
+      <c r="AX1" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="AW1" s="47" t="s">
+      <c r="AY1" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="AX1" s="47" t="s">
+      <c r="AZ1" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="BA1" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="AZ1" s="47" t="s">
+      <c r="BB1" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="BA1" s="47" t="s">
+      <c r="BC1" s="47" t="s">
         <v>163</v>
       </c>
-      <c r="BB1" s="47" t="s">
+      <c r="BD1" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="BC1" s="47" t="s">
+      <c r="BE1" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="BD1" s="47" t="s">
+      <c r="BF1" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="BE1" s="47" t="s">
+      <c r="BG1" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="BF1" s="47" t="s">
+      <c r="BH1" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="BG1" s="47" t="s">
+      <c r="BI1" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="BH1" s="47" t="s">
+      <c r="BJ1" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="BI1" s="47" t="s">
+      <c r="BK1" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="BJ1" s="47" t="s">
+      <c r="BL1" s="47" t="s">
         <v>172</v>
       </c>
-      <c r="BK1" s="47" t="s">
+      <c r="BM1" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="BL1" s="47" t="s">
+      <c r="BN1" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="BM1" s="47" t="s">
+      <c r="BO1" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="BN1" s="47" t="s">
+      <c r="BP1" s="47" t="s">
         <v>176</v>
       </c>
-      <c r="BO1" s="47" t="s">
+      <c r="BQ1" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="BP1" s="47" t="s">
+      <c r="BR1" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="BQ1" s="47" t="s">
+      <c r="BS1" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="BR1" s="47" t="s">
+      <c r="BT1" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="BS1" s="47" t="s">
+      <c r="BU1" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="BT1" s="47" t="s">
+      <c r="BV1" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="BU1" s="47" t="s">
+      <c r="BW1" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="BV1" s="47" t="s">
+      <c r="BX1" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="BW1" s="47" t="s">
+      <c r="BY1" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="BX1" s="47" t="s">
+      <c r="BZ1" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="BY1" s="47" t="s">
+      <c r="CA1" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="BZ1" s="47" t="s">
+      <c r="CB1" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="CA1" s="47" t="s">
+      <c r="CC1" s="47" t="s">
         <v>189</v>
       </c>
-      <c r="CB1" s="47" t="s">
+      <c r="CD1" s="47" t="s">
         <v>190</v>
       </c>
-      <c r="CC1" s="47" t="s">
+      <c r="CE1" s="47" t="s">
         <v>191</v>
       </c>
-      <c r="CD1" s="47" t="s">
+      <c r="CF1" s="47" t="s">
         <v>192</v>
       </c>
-      <c r="CE1" s="47" t="s">
+      <c r="CG1" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="CF1" s="47" t="s">
+      <c r="CH1" s="47" t="s">
         <v>194</v>
       </c>
-      <c r="CG1" s="47" t="s">
+      <c r="CI1" s="47" t="s">
         <v>195</v>
       </c>
-      <c r="CH1" s="47" t="s">
+      <c r="CJ1" s="47" t="s">
         <v>196</v>
       </c>
-      <c r="CI1" s="47" t="s">
+      <c r="CK1" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="CJ1" s="47" t="s">
+      <c r="CL1" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="CK1" s="47" t="s">
+      <c r="CM1" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="CL1" s="47" t="s">
+      <c r="CN1" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="CM1" s="47" t="s">
+      <c r="CO1" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="CN1" s="47" t="s">
+      <c r="CP1" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="CO1" s="47" t="s">
+      <c r="CQ1" s="47" t="s">
         <v>203</v>
       </c>
-      <c r="CP1" s="47" t="s">
+      <c r="CR1" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="CQ1" s="47" t="s">
+      <c r="CS1" s="47" t="s">
         <v>205</v>
       </c>
-      <c r="CR1" s="47" t="s">
+      <c r="CT1" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="CS1" s="47" t="s">
+      <c r="CU1" s="47" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:97" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>68</v>
       </c>
@@ -3171,67 +3184,73 @@
       <c r="AL2" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="AM2" s="25" t="s">
+      <c r="AM2" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="AN2" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="AN2" s="8" t="s">
+      <c r="AO2" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AP2" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="AP2" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="AQ2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AS2" s="66" t="s">
+      <c r="AR2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AT2" s="66" t="s">
         <v>231</v>
       </c>
-      <c r="AT2" s="8" t="s">
+      <c r="AU2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AU2" s="80" t="s">
+      <c r="AV2" s="80" t="s">
         <v>232</v>
       </c>
-      <c r="AV2" s="25" t="s">
+      <c r="AW2" s="80" t="s">
+        <v>397</v>
+      </c>
+      <c r="AX2" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="AX2" s="25" t="s">
+      <c r="AZ2" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="AY2" s="25" t="s">
+      <c r="BA2" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="AZ2" s="25" t="s">
+      <c r="BB2" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="BA2" s="8" t="s">
+      <c r="BC2" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="BB2" s="8" t="s">
+      <c r="BD2" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="BD2" s="25" t="s">
+      <c r="BF2" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="BE2" s="8" t="s">
+      <c r="BG2" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="BF2" s="56">
+      <c r="BH2" s="56">
         <v>43754</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BI2" t="s">
         <v>103</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CS2" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4147,8 +4166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4172,6 +4191,7 @@
     <col min="19" max="19" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24.28515625" style="24" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="21.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
@@ -4343,7 +4363,9 @@
       <c r="AD2" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="AE2" s="69"/>
+      <c r="AE2" s="69" t="s">
+        <v>397</v>
+      </c>
       <c r="AF2" s="69"/>
       <c r="AG2" s="69"/>
       <c r="AH2" s="70"/>

</xml_diff>

<commit_message>
GDE-9321 -update import file to add the new robot file -update the dataset -added optional argument ${sCycle_Frequency} in Update Commitment Fee Keyword -added writing of deal name, borrower name in sheet SERV08_ComprehensiveRepricing -added new robot file Repricing_New_Life_Bilat
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19638C6-ECBF-407A-99F3-CD4BD4926ABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0108339-124A-4B14-8D29-69A9D0C35173}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="CRED02_FacilitySetup" sheetId="3" r:id="rId3"/>
     <sheet name="CRED08_OngoingFeeSetup" sheetId="4" r:id="rId4"/>
     <sheet name="SERV29_CommitmentFeePayment" sheetId="5" r:id="rId5"/>
-    <sheet name="SYND02_PrimaryAllocation" sheetId="6" r:id="rId6"/>
-    <sheet name="SERV01_LoanDrawdown" sheetId="7" r:id="rId7"/>
-    <sheet name="Correspondence" sheetId="8" r:id="rId8"/>
+    <sheet name="SERV08_ComprehensiveRepricing" sheetId="6" r:id="rId6"/>
+    <sheet name="SYND02_PrimaryAllocation" sheetId="7" r:id="rId7"/>
+    <sheet name="SERV01_LoanDrawdown" sheetId="8" r:id="rId8"/>
+    <sheet name="Correspondence" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="513">
   <si>
     <t>rowid</t>
   </si>
@@ -668,13 +669,13 @@
     <t>NEW LIFE BILAT AUD 320M 14FEB2018_</t>
   </si>
   <si>
-    <t>NEW LIFE BILAT AUD 320M 14FEB2018_31124</t>
-  </si>
-  <si>
-    <t>31126</t>
-  </si>
-  <si>
-    <t>CLASS A DEBTHOLDERS43138</t>
+    <t>NEW LIFE BILAT AUD 320M 14FEB2018_04154</t>
+  </si>
+  <si>
+    <t>04155</t>
+  </si>
+  <si>
+    <t>CLASS A DEBTHOLDERS18132</t>
   </si>
   <si>
     <t>COMMONWEALTHBANKOFAUSTCB001</t>
@@ -1172,6 +1173,93 @@
     <t>14-Jan-2020</t>
   </si>
   <si>
+    <t>Amend_Commitment_Fee_21JAN2020</t>
+  </si>
+  <si>
+    <t>13-Feb-2025</t>
+  </si>
+  <si>
+    <t>to the actual due date</t>
+  </si>
+  <si>
+    <t>12-Feb-2025</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Amend_Commitment_Fee_19FEB2020</t>
+  </si>
+  <si>
+    <t>Amend_Commitment_Fee_19MAR2020</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Amend_Commitment_Fee_20APR2020</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Amend_Commitment_Fee_19MAY2020</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Amend_Commitment_Fee_19JUN2020</t>
+  </si>
+  <si>
+    <t>OutstandingSelect_Type</t>
+  </si>
+  <si>
+    <t>Loan_Alias</t>
+  </si>
+  <si>
+    <t>NewLoan_Alias</t>
+  </si>
+  <si>
+    <t>Borrower_Name</t>
+  </si>
+  <si>
+    <t>New_LoanAmount</t>
+  </si>
+  <si>
+    <t>Capitalize_PercentOfPayment</t>
+  </si>
+  <si>
+    <t>Repricing_Type</t>
+  </si>
+  <si>
+    <t>Repricing_Add_Option_Setup</t>
+  </si>
+  <si>
+    <t>Pricing_Option</t>
+  </si>
+  <si>
+    <t>Repricing_Frequency</t>
+  </si>
+  <si>
+    <t>AcceptRate_FromPricing</t>
+  </si>
+  <si>
+    <t>Base_Rate</t>
+  </si>
+  <si>
+    <t>60002124</t>
+  </si>
+  <si>
+    <t>Comprehensive Repricing</t>
+  </si>
+  <si>
+    <t>Rollover/Conversion to New:</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>Primary_Lender</t>
   </si>
   <si>
@@ -1247,18 +1335,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Loan_Alias</t>
-  </si>
-  <si>
-    <t>Borrower_Name</t>
-  </si>
-  <si>
     <t>Outstanding_Type</t>
   </si>
   <si>
-    <t>Pricing_Option</t>
-  </si>
-  <si>
     <t>Loan_RequestedAmount</t>
   </si>
   <si>
@@ -1283,9 +1362,6 @@
     <t>Loan_AccrualEndDate</t>
   </si>
   <si>
-    <t>AcceptRate_FromPricing</t>
-  </si>
-  <si>
     <t>RateSetting_NoticeStatus</t>
   </si>
   <si>
@@ -1316,9 +1392,6 @@
     <t>Loan_OverrideSpread</t>
   </si>
   <si>
-    <t>60002077</t>
-  </si>
-  <si>
     <t>191,569,254.72</t>
   </si>
   <si>
@@ -1328,9 +1401,6 @@
     <t>1 Months</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Awaiting release</t>
   </si>
   <si>
@@ -1493,43 +1563,10 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Amend_Commitment_Fee_21JAN2020</t>
-  </si>
-  <si>
-    <t>Amend_Commitment_Fee_19FEB2020</t>
-  </si>
-  <si>
-    <t>Amend_Commitment_Fee_19MAR2020</t>
-  </si>
-  <si>
-    <t>Amend_Commitment_Fee_20APR2020</t>
-  </si>
-  <si>
-    <t>Amend_Commitment_Fee_19MAY2020</t>
-  </si>
-  <si>
-    <t>Amend_Commitment_Fee_19JUN2020</t>
-  </si>
-  <si>
-    <t>13-Feb-2025</t>
-  </si>
-  <si>
-    <t>12-Feb-2025</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>to the actual due date</t>
+    <t>Commitment_CycleFrequency</t>
+  </si>
+  <si>
+    <t>Monthly</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1578,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000000000"/>
     <numFmt numFmtId="166" formatCode="00000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1628,6 +1665,18 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1748,7 +1797,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1906,6 +1955,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2774,7 +2844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CV2"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BH2" sqref="BH2"/>
     </sheetView>
   </sheetViews>
@@ -3840,11 +3910,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3857,20 +3925,25 @@
     <col min="8" max="8" width="29.85546875" style="24" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.140625" style="24" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="23" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" s="23" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -3902,79 +3975,82 @@
         <v>352</v>
       </c>
       <c r="K1" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="L1" s="23" t="s">
         <v>353</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="P1" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="Q1" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="R1" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="T1" s="23" t="s">
         <v>360</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="U1" s="48" t="s">
         <v>361</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="V1" s="48" t="s">
         <v>362</v>
       </c>
-      <c r="V1" s="48" t="s">
+      <c r="W1" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="W1" s="48" t="s">
+      <c r="X1" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="Y1" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Z1" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="AA1" s="20" t="s">
         <v>367</v>
       </c>
-      <c r="AA1" s="20" t="s">
+      <c r="AB1" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="AB1" s="20" t="s">
+      <c r="AC1" s="20" t="s">
         <v>369</v>
       </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AD1" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="AD1" s="23" t="s">
+      <c r="AE1" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="AE1" s="23" t="s">
+      <c r="AF1" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="AF1" s="23" t="s">
+      <c r="AG1" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="AG1" s="23" t="s">
+      <c r="AH1" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="AH1" s="23" t="s">
+      <c r="AI1" s="23" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>68</v>
       </c>
@@ -4005,53 +4081,54 @@
       <c r="J2" s="28" t="s">
         <v>380</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46" t="s">
+      <c r="K2" s="28"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="46"/>
-      <c r="N2" t="s">
+      <c r="N2" s="46"/>
+      <c r="O2" t="s">
         <v>96</v>
       </c>
-      <c r="O2" s="59" t="s">
+      <c r="P2" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="P2" s="66" t="s">
+      <c r="Q2" s="66" t="s">
         <v>218</v>
       </c>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="50"/>
+      <c r="R2" s="44"/>
       <c r="S2" s="50"/>
-      <c r="T2" s="44"/>
+      <c r="T2" s="50"/>
       <c r="U2" s="44"/>
       <c r="V2" s="44"/>
       <c r="W2" s="44"/>
-      <c r="X2" s="44">
-        <v>79169.64</v>
-      </c>
+      <c r="X2" s="44"/>
       <c r="Y2" s="44">
-        <v>0.75</v>
-      </c>
-      <c r="Z2" s="45">
+        <v>52779.76</v>
+      </c>
+      <c r="Z2" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="AA2" s="45">
         <v>128430745.28</v>
       </c>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="51">
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="51">
         <v>365</v>
       </c>
-      <c r="AC2" s="46"/>
       <c r="AD2" s="46"/>
-      <c r="AE2" s="52"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="52"/>
       <c r="AG2" s="52"/>
-      <c r="AH2" s="46"/>
+      <c r="AH2" s="52"/>
+      <c r="AI2" s="46"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>489</v>
+      <c r="B3" t="s">
+        <v>381</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>213</v>
@@ -4063,24 +4140,30 @@
         <v>215</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>495</v>
+        <v>382</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>283</v>
       </c>
-      <c r="I3" s="24" t="s">
-        <v>500</v>
+      <c r="I3" t="s">
+        <v>383</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>496</v>
+        <v>384</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>512</v>
+      </c>
+      <c r="O3" t="s">
+        <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>488</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>490</v>
+        <v>385</v>
+      </c>
+      <c r="B4" t="s">
+        <v>386</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>213</v>
@@ -4091,13 +4174,16 @@
       <c r="E4" s="8" t="s">
         <v>215</v>
       </c>
+      <c r="O4" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>491</v>
+      <c r="B5" t="s">
+        <v>387</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>213</v>
@@ -4108,13 +4194,16 @@
       <c r="E5" s="8" t="s">
         <v>215</v>
       </c>
+      <c r="O5" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>492</v>
+        <v>388</v>
+      </c>
+      <c r="B6" t="s">
+        <v>389</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>213</v>
@@ -4125,13 +4214,16 @@
       <c r="E6" s="8" t="s">
         <v>215</v>
       </c>
+      <c r="O6" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>493</v>
+        <v>390</v>
+      </c>
+      <c r="B7" t="s">
+        <v>391</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>213</v>
@@ -4142,13 +4234,16 @@
       <c r="E7" s="8" t="s">
         <v>215</v>
       </c>
+      <c r="O7" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>499</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>494</v>
+        <v>392</v>
+      </c>
+      <c r="B8" t="s">
+        <v>393</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>213</v>
@@ -4158,6 +4253,9 @@
       </c>
       <c r="E8" s="8" t="s">
         <v>215</v>
+      </c>
+      <c r="O8" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -4168,6 +4266,130 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" style="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>394</v>
+      </c>
+      <c r="E1" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="82" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1" s="82" t="s">
+        <v>396</v>
+      </c>
+      <c r="H1" s="83" t="s">
+        <v>397</v>
+      </c>
+      <c r="I1" s="84" t="s">
+        <v>398</v>
+      </c>
+      <c r="J1" s="84" t="s">
+        <v>399</v>
+      </c>
+      <c r="K1" s="81" t="s">
+        <v>400</v>
+      </c>
+      <c r="L1" s="81" t="s">
+        <v>401</v>
+      </c>
+      <c r="M1" s="81" t="s">
+        <v>402</v>
+      </c>
+      <c r="N1" s="81" t="s">
+        <v>403</v>
+      </c>
+      <c r="O1" s="64" t="s">
+        <v>404</v>
+      </c>
+      <c r="P1" s="81" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="85" t="s">
+        <v>284</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>406</v>
+      </c>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="86"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="85" t="s">
+        <v>407</v>
+      </c>
+      <c r="L2" s="85" t="s">
+        <v>408</v>
+      </c>
+      <c r="M2" s="85" t="s">
+        <v>225</v>
+      </c>
+      <c r="N2" s="87" t="s">
+        <v>456</v>
+      </c>
+      <c r="O2" s="59" t="s">
+        <v>409</v>
+      </c>
+      <c r="P2" s="87"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
@@ -4210,61 +4432,61 @@
         <v>117</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>381</v>
+        <v>410</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>382</v>
+        <v>411</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>383</v>
+        <v>412</v>
       </c>
       <c r="H1" s="47" t="s">
-        <v>384</v>
+        <v>413</v>
       </c>
       <c r="I1" s="47" t="s">
-        <v>385</v>
+        <v>414</v>
       </c>
       <c r="J1" s="47" t="s">
-        <v>386</v>
+        <v>415</v>
       </c>
       <c r="K1" s="47" t="s">
-        <v>387</v>
+        <v>416</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>388</v>
+        <v>417</v>
       </c>
       <c r="M1" s="47" t="s">
-        <v>389</v>
+        <v>418</v>
       </c>
       <c r="N1" s="47" t="s">
-        <v>390</v>
+        <v>419</v>
       </c>
       <c r="O1" s="47" t="s">
-        <v>391</v>
+        <v>420</v>
       </c>
       <c r="P1" s="47" t="s">
-        <v>392</v>
+        <v>421</v>
       </c>
       <c r="Q1" s="47" t="s">
-        <v>393</v>
+        <v>422</v>
       </c>
       <c r="R1" s="47" t="s">
-        <v>394</v>
+        <v>423</v>
       </c>
       <c r="S1" s="47" t="s">
-        <v>395</v>
+        <v>424</v>
       </c>
       <c r="T1" s="47" t="s">
-        <v>396</v>
+        <v>425</v>
       </c>
       <c r="U1" s="47" t="s">
-        <v>397</v>
+        <v>426</v>
       </c>
       <c r="V1" s="47" t="s">
-        <v>398</v>
+        <v>427</v>
       </c>
       <c r="W1" s="47" t="s">
-        <v>399</v>
+        <v>428</v>
       </c>
       <c r="Y1" s="47"/>
       <c r="Z1" s="47"/>
@@ -4294,16 +4516,16 @@
         <v>94</v>
       </c>
       <c r="G2" s="54" t="s">
-        <v>400</v>
+        <v>429</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>401</v>
+        <v>430</v>
       </c>
       <c r="I2" s="57" t="s">
-        <v>402</v>
+        <v>431</v>
       </c>
       <c r="J2" s="54" t="s">
-        <v>402</v>
+        <v>431</v>
       </c>
       <c r="K2" s="27" t="s">
         <v>217</v>
@@ -4318,11 +4540,11 @@
         <v>221</v>
       </c>
       <c r="O2" s="60" t="s">
-        <v>403</v>
+        <v>432</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="59" t="s">
-        <v>404</v>
+        <v>433</v>
       </c>
       <c r="R2" s="59" t="s">
         <v>89</v>
@@ -4335,7 +4557,7 @@
         <v>221</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>405</v>
+        <v>434</v>
       </c>
       <c r="W2" s="28" t="s">
         <v>221</v>
@@ -4355,12 +4577,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4401,40 +4623,40 @@
         <v>117</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="F1" s="63" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="G1" s="62" t="s">
-        <v>408</v>
+        <v>435</v>
       </c>
       <c r="H1" s="62" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="I1" s="62" t="s">
-        <v>410</v>
+        <v>436</v>
       </c>
       <c r="J1" s="62" t="s">
-        <v>411</v>
+        <v>437</v>
       </c>
       <c r="K1" s="64" t="s">
-        <v>412</v>
+        <v>438</v>
       </c>
       <c r="L1" s="62" t="s">
-        <v>413</v>
+        <v>439</v>
       </c>
       <c r="M1" s="62" t="s">
-        <v>414</v>
+        <v>440</v>
       </c>
       <c r="N1" s="62" t="s">
-        <v>415</v>
+        <v>441</v>
       </c>
       <c r="O1" s="62" t="s">
-        <v>416</v>
+        <v>442</v>
       </c>
       <c r="P1" s="62" t="s">
-        <v>417</v>
+        <v>443</v>
       </c>
       <c r="Q1" s="64" t="s">
         <v>357</v>
@@ -4443,16 +4665,16 @@
         <v>356</v>
       </c>
       <c r="S1" s="64" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="T1" s="64" t="s">
-        <v>419</v>
+        <v>444</v>
       </c>
       <c r="U1" s="63" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="V1" s="63" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="W1" s="63" t="s">
         <v>361</v>
@@ -4467,25 +4689,25 @@
         <v>364</v>
       </c>
       <c r="AA1" s="63" t="s">
-        <v>422</v>
+        <v>447</v>
       </c>
       <c r="AB1" s="63" t="s">
-        <v>423</v>
+        <v>448</v>
       </c>
       <c r="AC1" s="63" t="s">
-        <v>424</v>
+        <v>449</v>
       </c>
       <c r="AD1" s="62" t="s">
-        <v>425</v>
+        <v>450</v>
       </c>
       <c r="AE1" s="62" t="s">
-        <v>426</v>
+        <v>451</v>
       </c>
       <c r="AF1" s="62" t="s">
-        <v>427</v>
+        <v>452</v>
       </c>
       <c r="AG1" s="62" t="s">
-        <v>428</v>
+        <v>453</v>
       </c>
       <c r="AH1" s="62"/>
     </row>
@@ -4503,7 +4725,7 @@
         <v>215</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="F2" s="59" t="s">
         <v>96</v>
@@ -4515,16 +4737,16 @@
         <v>225</v>
       </c>
       <c r="I2" s="65" t="s">
-        <v>430</v>
+        <v>454</v>
       </c>
       <c r="J2" s="66" t="s">
-        <v>431</v>
+        <v>455</v>
       </c>
       <c r="K2" s="60" t="s">
         <v>283</v>
       </c>
       <c r="L2" s="59" t="s">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="M2" s="67" t="s">
         <v>231</v>
@@ -4539,10 +4761,10 @@
       <c r="Q2" s="59"/>
       <c r="R2" s="59"/>
       <c r="S2" s="59" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="T2" s="59" t="s">
-        <v>434</v>
+        <v>457</v>
       </c>
       <c r="U2" s="68"/>
       <c r="V2" s="68"/>
@@ -4568,8 +4790,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:BL4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4592,103 +4814,103 @@
         <v>117</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>435</v>
+        <v>458</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="H1" s="72" t="s">
-        <v>437</v>
+        <v>460</v>
       </c>
       <c r="I1" s="72" t="s">
-        <v>438</v>
+        <v>461</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>439</v>
+        <v>462</v>
       </c>
       <c r="K1" s="72" t="s">
-        <v>440</v>
+        <v>463</v>
       </c>
       <c r="L1" s="72" t="s">
-        <v>441</v>
+        <v>464</v>
       </c>
       <c r="M1" s="72" t="s">
-        <v>442</v>
+        <v>465</v>
       </c>
       <c r="N1" s="72" t="s">
-        <v>443</v>
+        <v>466</v>
       </c>
       <c r="O1" s="71" t="s">
-        <v>444</v>
+        <v>467</v>
       </c>
       <c r="P1" s="72" t="s">
-        <v>445</v>
+        <v>468</v>
       </c>
       <c r="Q1" s="72" t="s">
-        <v>446</v>
+        <v>469</v>
       </c>
       <c r="R1" s="72" t="s">
-        <v>447</v>
+        <v>470</v>
       </c>
       <c r="S1" s="71" t="s">
-        <v>448</v>
+        <v>471</v>
       </c>
       <c r="T1" s="71" t="s">
-        <v>449</v>
+        <v>472</v>
       </c>
       <c r="U1" s="71" t="s">
-        <v>450</v>
+        <v>473</v>
       </c>
       <c r="V1" s="71" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="W1" s="71" t="s">
-        <v>452</v>
+        <v>475</v>
       </c>
       <c r="X1" s="71" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="Y1" s="71" t="s">
-        <v>454</v>
+        <v>477</v>
       </c>
       <c r="Z1" s="71" t="s">
-        <v>455</v>
+        <v>478</v>
       </c>
       <c r="AA1" s="71" t="s">
-        <v>456</v>
+        <v>479</v>
       </c>
       <c r="AB1" s="71" t="s">
-        <v>457</v>
+        <v>480</v>
       </c>
       <c r="AC1" s="74" t="s">
-        <v>458</v>
+        <v>481</v>
       </c>
       <c r="AD1" s="74" t="s">
-        <v>459</v>
+        <v>482</v>
       </c>
       <c r="AE1" s="74" t="s">
-        <v>460</v>
+        <v>483</v>
       </c>
       <c r="AF1" s="75" t="s">
-        <v>461</v>
+        <v>484</v>
       </c>
       <c r="AG1" s="74" t="s">
-        <v>462</v>
+        <v>485</v>
       </c>
       <c r="AH1" s="71" t="s">
-        <v>463</v>
+        <v>486</v>
       </c>
       <c r="AI1" s="71" t="s">
-        <v>464</v>
+        <v>487</v>
       </c>
       <c r="AJ1" s="76" t="s">
-        <v>465</v>
+        <v>488</v>
       </c>
       <c r="AK1" s="76" t="s">
-        <v>466</v>
+        <v>489</v>
       </c>
       <c r="AL1" s="76" t="s">
         <v>291</v>
@@ -4700,76 +4922,76 @@
         <v>369</v>
       </c>
       <c r="AO1" s="71" t="s">
-        <v>467</v>
+        <v>490</v>
       </c>
       <c r="AP1" s="72" t="s">
-        <v>468</v>
+        <v>491</v>
       </c>
       <c r="AQ1" s="72" t="s">
-        <v>469</v>
+        <v>492</v>
       </c>
       <c r="AR1" s="72" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="AS1" s="72" t="s">
-        <v>471</v>
+        <v>494</v>
       </c>
       <c r="AT1" s="72" t="s">
-        <v>411</v>
+        <v>437</v>
       </c>
       <c r="AU1" s="72" t="s">
-        <v>412</v>
+        <v>438</v>
       </c>
       <c r="AV1" s="72" t="s">
-        <v>472</v>
+        <v>495</v>
       </c>
       <c r="AW1" s="72" t="s">
-        <v>473</v>
+        <v>496</v>
       </c>
       <c r="AX1" s="72" t="s">
-        <v>416</v>
+        <v>442</v>
       </c>
       <c r="AY1" s="72" t="s">
-        <v>474</v>
+        <v>497</v>
       </c>
       <c r="AZ1" s="71" t="s">
-        <v>475</v>
+        <v>498</v>
       </c>
       <c r="BA1" s="72" t="s">
-        <v>476</v>
+        <v>499</v>
       </c>
       <c r="BB1" s="72" t="s">
-        <v>477</v>
+        <v>500</v>
       </c>
       <c r="BC1" s="71" t="s">
-        <v>478</v>
+        <v>501</v>
       </c>
       <c r="BD1" s="71" t="s">
-        <v>479</v>
+        <v>502</v>
       </c>
       <c r="BE1" s="71" t="s">
-        <v>480</v>
+        <v>503</v>
       </c>
       <c r="BF1" s="71" t="s">
-        <v>481</v>
+        <v>504</v>
       </c>
       <c r="BG1" s="71" t="s">
-        <v>482</v>
+        <v>505</v>
       </c>
       <c r="BH1" s="71" t="s">
-        <v>483</v>
+        <v>506</v>
       </c>
       <c r="BI1" s="71" t="s">
-        <v>484</v>
+        <v>507</v>
       </c>
       <c r="BJ1" s="71" t="s">
-        <v>485</v>
+        <v>508</v>
       </c>
       <c r="BK1" s="71" t="s">
-        <v>486</v>
+        <v>509</v>
       </c>
       <c r="BL1" s="72" t="s">
-        <v>487</v>
+        <v>510</v>
       </c>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.2">
@@ -4777,7 +4999,7 @@
         <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.2">
@@ -4785,15 +5007,15 @@
         <v>236</v>
       </c>
       <c r="E3" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A4" s="78" t="s">
-        <v>488</v>
+        <v>385</v>
       </c>
       <c r="E4" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-rename the test cases to be more specific -rename the robot file since its missing 0 on its file name -added another robot file for this ticket. -updated dataset
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -3207,8 +3207,8 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3569,6 +3569,11 @@
           <t>Monthly</t>
         </is>
       </c>
+      <c r="M3" s="46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="O3" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
@@ -3601,10 +3606,38 @@
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
+      <c r="F4" s="28" t="n"/>
+      <c r="H4" s="28" t="inlineStr">
+        <is>
+          <t>19-Feb-2020</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="M4" s="46" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="O4" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
+      </c>
+      <c r="Y4" t="n">
+        <v>59538.71</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>124180745.28</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>365</v>
       </c>
     </row>
     <row r="5">
@@ -3633,6 +3666,7 @@
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
+      <c r="M5" s="46" t="n"/>
       <c r="O5" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
@@ -4245,7 +4279,7 @@
   </sheetPr>
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GDE-9383 -updated dataset -remove writing of Loan_Alias in SERV08_ComprehensiveRepricing sheet -added new keyword Loan combine and rollover -rename TC to be more specific
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0BCA86-76AE-4ADE-B632-153CD79B09E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6E0092-9049-4F42-AB46-021C9F181DEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="3210" windowWidth="21600" windowHeight="11385" tabRatio="877" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,27 @@
     <sheet name="CRED02_FacilitySetup" sheetId="3" r:id="rId3"/>
     <sheet name="CRED08_OngoingFeeSetup" sheetId="4" r:id="rId4"/>
     <sheet name="SERV29_CommitmentFeePayment" sheetId="5" r:id="rId5"/>
-    <sheet name="SERV08_ComprehensiveRepricing" sheetId="6" r:id="rId6"/>
-    <sheet name="SYND02_PrimaryAllocation" sheetId="7" r:id="rId7"/>
-    <sheet name="SERV01_LoanDrawdown" sheetId="8" r:id="rId8"/>
+    <sheet name="SERV01_LoanDrawdown" sheetId="6" r:id="rId6"/>
+    <sheet name="SERV08_ComprehensiveRepricing" sheetId="7" r:id="rId7"/>
+    <sheet name="SYND02_PrimaryAllocation" sheetId="8" r:id="rId8"/>
     <sheet name="Correspondence" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="526">
   <si>
     <t>rowid</t>
   </si>
@@ -1176,67 +1186,169 @@
     <t>14-Jan-2020</t>
   </si>
   <si>
+    <t>Collect_Commitment_Fee_21JAN2020</t>
+  </si>
+  <si>
+    <t>13-Feb-2025</t>
+  </si>
+  <si>
+    <t>to the actual due date</t>
+  </si>
+  <si>
+    <t>12-Feb-2025</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Amend_Commitment_Fee_21JAN2020</t>
   </si>
   <si>
-    <t>13-Feb-2025</t>
-  </si>
-  <si>
-    <t>to the actual due date</t>
-  </si>
-  <si>
-    <t>12-Feb-2025</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Collect_Commitment_Fee_19FEB2020</t>
   </si>
   <si>
     <t>19-Feb-2020</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Amend_Commitment_Fee_19FEB2020</t>
   </si>
   <si>
-    <t>5</t>
+    <t>16-Mar-2025</t>
+  </si>
+  <si>
+    <t>19-Mar-2025</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>Amend_Commitment_Fee_19MAR2020</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>Amend_Commitment_Fee_20APR2020</t>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>Amend_Commitment_Fee_19MAY2020</t>
   </si>
   <si>
-    <t>8</t>
+    <t>9</t>
   </si>
   <si>
     <t>Amend_Commitment_Fee_19JUN2020</t>
   </si>
   <si>
+    <t>Loan_Alias</t>
+  </si>
+  <si>
+    <t>Borrower_Name</t>
+  </si>
+  <si>
+    <t>Outstanding_Type</t>
+  </si>
+  <si>
+    <t>Pricing_Option</t>
+  </si>
+  <si>
+    <t>Loan_RequestedAmount</t>
+  </si>
+  <si>
+    <t>Loan_EffectiveDate</t>
+  </si>
+  <si>
+    <t>Loan_MaturityDate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingFrequency</t>
+  </si>
+  <si>
+    <t>Loan_IntCycleFrequency</t>
+  </si>
+  <si>
+    <t>Loan_Accrue</t>
+  </si>
+  <si>
+    <t>Loan_RepricingDate</t>
+  </si>
+  <si>
+    <t>Loan_AccrualEndDate</t>
+  </si>
+  <si>
+    <t>AcceptRate_FromPricing</t>
+  </si>
+  <si>
+    <t>RateSetting_NoticeStatus</t>
+  </si>
+  <si>
+    <t>Lender</t>
+  </si>
+  <si>
+    <t>Lender2</t>
+  </si>
+  <si>
+    <t>HostBank_LenderShare</t>
+  </si>
+  <si>
+    <t>Lender1_Share</t>
+  </si>
+  <si>
+    <t>Lender2_Share</t>
+  </si>
+  <si>
+    <t>Outstanding_Currency</t>
+  </si>
+  <si>
+    <t>Loan_BorrowerBaseRate</t>
+  </si>
+  <si>
+    <t>Loan_FacilitySpread</t>
+  </si>
+  <si>
+    <t>Loan_OverrideSpread</t>
+  </si>
+  <si>
+    <t>60002197</t>
+  </si>
+  <si>
+    <t>191,569,254.72</t>
+  </si>
+  <si>
+    <t>19-Dec-2019</t>
+  </si>
+  <si>
+    <t>1 Months</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Awaiting release</t>
+  </si>
+  <si>
+    <t>60002225</t>
+  </si>
+  <si>
+    <t>4,250,000.00</t>
+  </si>
+  <si>
     <t>OutstandingSelect_Type</t>
   </si>
   <si>
-    <t>Loan_Alias</t>
-  </si>
-  <si>
     <t>NewLoan_Alias</t>
   </si>
   <si>
-    <t>Borrower_Name</t>
+    <t>CombineExistingLoans</t>
   </si>
   <si>
     <t>New_LoanAmount</t>
@@ -1251,21 +1363,12 @@
     <t>Repricing_Add_Option_Setup</t>
   </si>
   <si>
-    <t>Pricing_Option</t>
-  </si>
-  <si>
     <t>Repricing_Frequency</t>
   </si>
   <si>
-    <t>AcceptRate_FromPricing</t>
-  </si>
-  <si>
     <t>Base_Rate</t>
   </si>
   <si>
-    <t>60002197</t>
-  </si>
-  <si>
     <t>60002220</t>
   </si>
   <si>
@@ -1275,13 +1378,7 @@
     <t>Rollover/Conversion to New:</t>
   </si>
   <si>
-    <t>1 Months</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>60002225</t>
+    <t>60002309</t>
   </si>
   <si>
     <t>Primary_Lender</t>
@@ -1359,75 +1456,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Outstanding_Type</t>
-  </si>
-  <si>
-    <t>Loan_RequestedAmount</t>
-  </si>
-  <si>
-    <t>Loan_EffectiveDate</t>
-  </si>
-  <si>
-    <t>Loan_MaturityDate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingFrequency</t>
-  </si>
-  <si>
-    <t>Loan_IntCycleFrequency</t>
-  </si>
-  <si>
-    <t>Loan_Accrue</t>
-  </si>
-  <si>
-    <t>Loan_RepricingDate</t>
-  </si>
-  <si>
-    <t>Loan_AccrualEndDate</t>
-  </si>
-  <si>
-    <t>RateSetting_NoticeStatus</t>
-  </si>
-  <si>
-    <t>Lender</t>
-  </si>
-  <si>
-    <t>Lender2</t>
-  </si>
-  <si>
-    <t>HostBank_LenderShare</t>
-  </si>
-  <si>
-    <t>Lender1_Share</t>
-  </si>
-  <si>
-    <t>Lender2_Share</t>
-  </si>
-  <si>
-    <t>Outstanding_Currency</t>
-  </si>
-  <si>
-    <t>Loan_BorrowerBaseRate</t>
-  </si>
-  <si>
-    <t>Loan_FacilitySpread</t>
-  </si>
-  <si>
-    <t>Loan_OverrideSpread</t>
-  </si>
-  <si>
-    <t>191,569,254.72</t>
-  </si>
-  <si>
-    <t>19-Dec-2019</t>
-  </si>
-  <si>
-    <t>Awaiting release</t>
-  </si>
-  <si>
-    <t>4,250,000.00</t>
-  </si>
-  <si>
     <t>SubAdd_Days</t>
   </si>
   <si>
@@ -1587,16 +1615,7 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>16-Mar-2025</t>
-  </si>
-  <si>
-    <t>19-Mar-2025</t>
-  </si>
-  <si>
-    <t>Collect_Commitment_Fee_21JAN2020</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>19Feb2021_CombineAndRollover</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1816,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1820,6 +1839,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1827,7 +1855,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2009,6 +2037,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -3943,8 +3975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4156,12 +4188,12 @@
       <c r="AH2" s="52"/>
       <c r="AI2" s="46"/>
     </row>
-    <row r="3" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>521</v>
+      <c r="B3" t="s">
+        <v>382</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>213</v>
@@ -4178,7 +4210,7 @@
       <c r="H3" s="28" t="s">
         <v>283</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" t="s">
         <v>384</v>
       </c>
       <c r="J3" s="28" t="s">
@@ -4190,7 +4222,7 @@
       <c r="M3" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4199,7 +4231,7 @@
         <v>387</v>
       </c>
       <c r="B4" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>213</v>
@@ -4237,7 +4269,7 @@
         <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>213</v>
@@ -4250,7 +4282,7 @@
       </c>
       <c r="F5" s="28"/>
       <c r="H5" s="28" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I5" t="s">
         <v>384</v>
@@ -4279,7 +4311,7 @@
         <v>391</v>
       </c>
       <c r="B6" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>213</v>
@@ -4294,10 +4326,10 @@
         <v>377</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>519</v>
+        <v>393</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>520</v>
+        <v>394</v>
       </c>
       <c r="I6" t="s">
         <v>384</v>
@@ -4324,10 +4356,10 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B7" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>213</v>
@@ -4345,10 +4377,10 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B8" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>213</v>
@@ -4365,10 +4397,10 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B9" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>213</v>
@@ -4385,10 +4417,10 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>522</v>
+        <v>401</v>
       </c>
       <c r="B10" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>213</v>
@@ -4411,141 +4443,277 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.7109375" style="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="81" t="s">
-        <v>399</v>
-      </c>
-      <c r="E1" s="82" t="s">
+      <c r="D1" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="82" t="s">
-        <v>400</v>
-      </c>
-      <c r="G1" s="82" t="s">
-        <v>401</v>
-      </c>
-      <c r="H1" s="83" t="s">
-        <v>402</v>
-      </c>
-      <c r="I1" s="84" t="s">
+      <c r="E1" s="63" t="s">
         <v>403</v>
       </c>
-      <c r="J1" s="84" t="s">
+      <c r="F1" s="63" t="s">
         <v>404</v>
       </c>
-      <c r="K1" s="81" t="s">
+      <c r="G1" s="62" t="s">
         <v>405</v>
       </c>
-      <c r="L1" s="81" t="s">
+      <c r="H1" s="62" t="s">
         <v>406</v>
       </c>
-      <c r="M1" s="81" t="s">
+      <c r="I1" s="62" t="s">
         <v>407</v>
       </c>
-      <c r="N1" s="81" t="s">
+      <c r="J1" s="62" t="s">
         <v>408</v>
       </c>
-      <c r="O1" s="64" t="s">
+      <c r="K1" s="64" t="s">
         <v>409</v>
       </c>
-      <c r="P1" s="81" t="s">
+      <c r="L1" s="62" t="s">
         <v>410</v>
       </c>
+      <c r="M1" s="62" t="s">
+        <v>411</v>
+      </c>
+      <c r="N1" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="O1" s="62" t="s">
+        <v>413</v>
+      </c>
+      <c r="P1" s="62" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q1" s="64" t="s">
+        <v>358</v>
+      </c>
+      <c r="R1" s="64" t="s">
+        <v>357</v>
+      </c>
+      <c r="S1" s="64" t="s">
+        <v>415</v>
+      </c>
+      <c r="T1" s="64" t="s">
+        <v>416</v>
+      </c>
+      <c r="U1" s="63" t="s">
+        <v>417</v>
+      </c>
+      <c r="V1" s="63" t="s">
+        <v>418</v>
+      </c>
+      <c r="W1" s="63" t="s">
+        <v>362</v>
+      </c>
+      <c r="X1" s="63" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y1" s="63" t="s">
+        <v>364</v>
+      </c>
+      <c r="Z1" s="63" t="s">
+        <v>365</v>
+      </c>
+      <c r="AA1" s="63" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB1" s="63" t="s">
+        <v>420</v>
+      </c>
+      <c r="AC1" s="63" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD1" s="62" t="s">
+        <v>422</v>
+      </c>
+      <c r="AE1" s="62" t="s">
+        <v>423</v>
+      </c>
+      <c r="AF1" s="62" t="s">
+        <v>424</v>
+      </c>
+      <c r="AG1" s="62" t="s">
+        <v>425</v>
+      </c>
+      <c r="AH1" s="62"/>
     </row>
-    <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="8" t="s">
         <v>211</v>
       </c>
       <c r="C2" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>426</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="59" t="s">
         <v>284</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="H2" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="I2" s="65" t="s">
+        <v>427</v>
+      </c>
+      <c r="J2" s="66" t="s">
+        <v>428</v>
+      </c>
+      <c r="K2" s="60" t="s">
+        <v>283</v>
+      </c>
+      <c r="L2" s="59" t="s">
+        <v>429</v>
+      </c>
+      <c r="M2" s="67" t="s">
+        <v>231</v>
+      </c>
+      <c r="N2" s="59" t="s">
+        <v>380</v>
+      </c>
+      <c r="O2" s="66" t="s">
+        <v>379</v>
+      </c>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59" t="s">
+        <v>430</v>
+      </c>
+      <c r="T2" s="59" t="s">
+        <v>431</v>
+      </c>
+      <c r="U2" s="68"/>
+      <c r="V2" s="68"/>
+      <c r="W2" s="69"/>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="69"/>
+      <c r="Z2" s="69"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE2" s="69" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="70"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" s="53" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="59" t="s">
-        <v>411</v>
-      </c>
-      <c r="G2" s="59" t="s">
-        <v>412</v>
-      </c>
-      <c r="H2" s="59" t="s">
+      <c r="E3" s="59" t="s">
+        <v>432</v>
+      </c>
+      <c r="F3" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="86"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="85" t="s">
-        <v>413</v>
-      </c>
-      <c r="L2" s="85" t="s">
-        <v>414</v>
-      </c>
-      <c r="M2" s="85" t="s">
+      <c r="G3" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="H3" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="N2" s="87" t="s">
-        <v>415</v>
-      </c>
-      <c r="O2" s="59" t="s">
-        <v>416</v>
-      </c>
-      <c r="P2" s="87"/>
+      <c r="I3" s="65" t="s">
+        <v>433</v>
+      </c>
+      <c r="J3" s="88">
+        <v>43858</v>
+      </c>
+      <c r="K3" s="60" t="s">
+        <v>283</v>
+      </c>
+      <c r="L3" s="59" t="s">
+        <v>429</v>
+      </c>
+      <c r="N3" s="59" t="s">
+        <v>380</v>
+      </c>
+      <c r="O3" s="66" t="s">
+        <v>390</v>
+      </c>
+      <c r="P3" s="88">
+        <v>43879</v>
+      </c>
+      <c r="S3" s="59" t="s">
+        <v>430</v>
+      </c>
+      <c r="T3" s="59" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD3" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE3" s="69" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="C3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F3" t="s">
-        <v>417</v>
-      </c>
-      <c r="H3" t="s">
-        <v>96</v>
-      </c>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4" s="53"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="44"/>
+      <c r="F4" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4554,6 +4722,178 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>434</v>
+      </c>
+      <c r="E1" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="82" t="s">
+        <v>403</v>
+      </c>
+      <c r="G1" s="82" t="s">
+        <v>435</v>
+      </c>
+      <c r="H1" s="82" t="s">
+        <v>436</v>
+      </c>
+      <c r="I1" s="83" t="s">
+        <v>404</v>
+      </c>
+      <c r="J1" s="84" t="s">
+        <v>437</v>
+      </c>
+      <c r="K1" s="84" t="s">
+        <v>438</v>
+      </c>
+      <c r="L1" s="81" t="s">
+        <v>439</v>
+      </c>
+      <c r="M1" s="81" t="s">
+        <v>440</v>
+      </c>
+      <c r="N1" s="81" t="s">
+        <v>406</v>
+      </c>
+      <c r="O1" s="81" t="s">
+        <v>441</v>
+      </c>
+      <c r="P1" s="64" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q1" s="81" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="85" t="s">
+        <v>284</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>426</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>443</v>
+      </c>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="85" t="s">
+        <v>444</v>
+      </c>
+      <c r="M2" s="85" t="s">
+        <v>445</v>
+      </c>
+      <c r="N2" s="85" t="s">
+        <v>225</v>
+      </c>
+      <c r="O2" s="87" t="s">
+        <v>429</v>
+      </c>
+      <c r="P2" s="59" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q2" s="87"/>
+    </row>
+    <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="F3" s="89"/>
+      <c r="G3" t="s">
+        <v>446</v>
+      </c>
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT(G2,",",SERV01_LoanDrawdown!E3)</f>
+        <v>60002220,60002225</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" s="85" t="s">
+        <v>444</v>
+      </c>
+      <c r="M3" s="85" t="s">
+        <v>445</v>
+      </c>
+      <c r="N3" s="85" t="s">
+        <v>225</v>
+      </c>
+      <c r="O3" s="87" t="s">
+        <v>429</v>
+      </c>
+      <c r="P3" s="90" t="s">
+        <v>430</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4596,61 +4936,61 @@
         <v>117</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>418</v>
+        <v>447</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>420</v>
+        <v>449</v>
       </c>
       <c r="H1" s="47" t="s">
-        <v>421</v>
+        <v>450</v>
       </c>
       <c r="I1" s="47" t="s">
-        <v>422</v>
+        <v>451</v>
       </c>
       <c r="J1" s="47" t="s">
-        <v>423</v>
+        <v>452</v>
       </c>
       <c r="K1" s="47" t="s">
-        <v>424</v>
+        <v>453</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>425</v>
+        <v>454</v>
       </c>
       <c r="M1" s="47" t="s">
-        <v>426</v>
+        <v>455</v>
       </c>
       <c r="N1" s="47" t="s">
-        <v>427</v>
+        <v>456</v>
       </c>
       <c r="O1" s="47" t="s">
-        <v>428</v>
+        <v>457</v>
       </c>
       <c r="P1" s="47" t="s">
-        <v>429</v>
+        <v>458</v>
       </c>
       <c r="Q1" s="47" t="s">
-        <v>430</v>
+        <v>459</v>
       </c>
       <c r="R1" s="47" t="s">
-        <v>431</v>
+        <v>460</v>
       </c>
       <c r="S1" s="47" t="s">
-        <v>432</v>
+        <v>461</v>
       </c>
       <c r="T1" s="47" t="s">
-        <v>433</v>
+        <v>462</v>
       </c>
       <c r="U1" s="47" t="s">
-        <v>434</v>
+        <v>463</v>
       </c>
       <c r="V1" s="47" t="s">
-        <v>435</v>
+        <v>464</v>
       </c>
       <c r="W1" s="47" t="s">
-        <v>436</v>
+        <v>465</v>
       </c>
       <c r="Y1" s="47"/>
       <c r="Z1" s="47"/>
@@ -4680,16 +5020,16 @@
         <v>94</v>
       </c>
       <c r="G2" s="54" t="s">
-        <v>437</v>
+        <v>466</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>438</v>
+        <v>467</v>
       </c>
       <c r="I2" s="57" t="s">
-        <v>439</v>
+        <v>468</v>
       </c>
       <c r="J2" s="54" t="s">
-        <v>439</v>
+        <v>468</v>
       </c>
       <c r="K2" s="27" t="s">
         <v>217</v>
@@ -4704,11 +5044,11 @@
         <v>221</v>
       </c>
       <c r="O2" s="60" t="s">
-        <v>440</v>
+        <v>469</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="59" t="s">
-        <v>441</v>
+        <v>470</v>
       </c>
       <c r="R2" s="59" t="s">
         <v>89</v>
@@ -4721,7 +5061,7 @@
         <v>221</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>442</v>
+        <v>471</v>
       </c>
       <c r="W2" s="28" t="s">
         <v>221</v>
@@ -4738,278 +5078,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AH3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="21.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24" style="24" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="63" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" s="63" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="63" t="s">
-        <v>400</v>
-      </c>
-      <c r="F1" s="63" t="s">
-        <v>402</v>
-      </c>
-      <c r="G1" s="62" t="s">
-        <v>443</v>
-      </c>
-      <c r="H1" s="62" t="s">
-        <v>407</v>
-      </c>
-      <c r="I1" s="62" t="s">
-        <v>444</v>
-      </c>
-      <c r="J1" s="62" t="s">
-        <v>445</v>
-      </c>
-      <c r="K1" s="64" t="s">
-        <v>446</v>
-      </c>
-      <c r="L1" s="62" t="s">
-        <v>447</v>
-      </c>
-      <c r="M1" s="62" t="s">
-        <v>448</v>
-      </c>
-      <c r="N1" s="62" t="s">
-        <v>449</v>
-      </c>
-      <c r="O1" s="62" t="s">
-        <v>450</v>
-      </c>
-      <c r="P1" s="62" t="s">
-        <v>451</v>
-      </c>
-      <c r="Q1" s="64" t="s">
-        <v>358</v>
-      </c>
-      <c r="R1" s="64" t="s">
-        <v>357</v>
-      </c>
-      <c r="S1" s="64" t="s">
-        <v>409</v>
-      </c>
-      <c r="T1" s="64" t="s">
-        <v>452</v>
-      </c>
-      <c r="U1" s="63" t="s">
-        <v>453</v>
-      </c>
-      <c r="V1" s="63" t="s">
-        <v>454</v>
-      </c>
-      <c r="W1" s="63" t="s">
-        <v>362</v>
-      </c>
-      <c r="X1" s="63" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y1" s="63" t="s">
-        <v>364</v>
-      </c>
-      <c r="Z1" s="63" t="s">
-        <v>365</v>
-      </c>
-      <c r="AA1" s="63" t="s">
-        <v>455</v>
-      </c>
-      <c r="AB1" s="63" t="s">
-        <v>456</v>
-      </c>
-      <c r="AC1" s="63" t="s">
-        <v>457</v>
-      </c>
-      <c r="AD1" s="62" t="s">
-        <v>458</v>
-      </c>
-      <c r="AE1" s="62" t="s">
-        <v>459</v>
-      </c>
-      <c r="AF1" s="62" t="s">
-        <v>460</v>
-      </c>
-      <c r="AG1" s="62" t="s">
-        <v>461</v>
-      </c>
-      <c r="AH1" s="62"/>
-    </row>
-    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>411</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="59" t="s">
-        <v>284</v>
-      </c>
-      <c r="H2" s="59" t="s">
-        <v>225</v>
-      </c>
-      <c r="I2" s="65" t="s">
-        <v>462</v>
-      </c>
-      <c r="J2" s="66" t="s">
-        <v>463</v>
-      </c>
-      <c r="K2" s="60" t="s">
-        <v>283</v>
-      </c>
-      <c r="L2" s="59" t="s">
-        <v>415</v>
-      </c>
-      <c r="M2" s="67" t="s">
-        <v>231</v>
-      </c>
-      <c r="N2" s="59" t="s">
-        <v>380</v>
-      </c>
-      <c r="O2" s="66" t="s">
-        <v>379</v>
-      </c>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59" t="s">
-        <v>416</v>
-      </c>
-      <c r="T2" s="59" t="s">
-        <v>464</v>
-      </c>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE2" s="69" t="s">
-        <v>231</v>
-      </c>
-      <c r="AF2" s="69"/>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="70"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
-        <v>236</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>417</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>284</v>
-      </c>
-      <c r="H3" s="59" t="s">
-        <v>225</v>
-      </c>
-      <c r="I3" s="65" t="s">
-        <v>465</v>
-      </c>
-      <c r="J3" s="88">
-        <v>43858</v>
-      </c>
-      <c r="K3" s="60" t="s">
-        <v>283</v>
-      </c>
-      <c r="L3" s="59" t="s">
-        <v>415</v>
-      </c>
-      <c r="N3" s="59" t="s">
-        <v>380</v>
-      </c>
-      <c r="O3" s="66" t="s">
-        <v>389</v>
-      </c>
-      <c r="P3" s="88">
-        <v>43879</v>
-      </c>
-      <c r="S3" s="59" t="s">
-        <v>416</v>
-      </c>
-      <c r="T3" s="59" t="s">
-        <v>464</v>
-      </c>
-      <c r="AD3" s="69" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE3" s="69" t="s">
-        <v>231</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5037,103 +5105,103 @@
         <v>117</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="H1" s="72" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="I1" s="72" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="K1" s="72" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="L1" s="72" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="M1" s="72" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="N1" s="72" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="O1" s="71" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="P1" s="72" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="Q1" s="72" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="R1" s="72" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="S1" s="71" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="T1" s="71" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="U1" s="71" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="V1" s="71" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="W1" s="71" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="X1" s="71" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="Y1" s="71" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="Z1" s="71" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="AA1" s="71" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="AB1" s="71" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="AC1" s="74" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="AD1" s="74" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="AE1" s="74" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="AF1" s="75" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="AG1" s="74" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="AH1" s="71" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="AI1" s="71" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="AJ1" s="76" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="AK1" s="76" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="AL1" s="76" t="s">
         <v>291</v>
@@ -5145,76 +5213,76 @@
         <v>370</v>
       </c>
       <c r="AO1" s="71" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="AP1" s="72" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="AQ1" s="72" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="AR1" s="72" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="AS1" s="72" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="AT1" s="72" t="s">
-        <v>445</v>
+        <v>408</v>
       </c>
       <c r="AU1" s="72" t="s">
-        <v>446</v>
+        <v>409</v>
       </c>
       <c r="AV1" s="72" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="AW1" s="72" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="AX1" s="72" t="s">
-        <v>450</v>
+        <v>413</v>
       </c>
       <c r="AY1" s="72" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="AZ1" s="71" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="BA1" s="72" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="BB1" s="72" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="BC1" s="71" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="BD1" s="71" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="BE1" s="71" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="BF1" s="71" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="BG1" s="71" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="BH1" s="71" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="BI1" s="71" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="BJ1" s="71" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="BK1" s="71" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="BL1" s="72" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.2">
@@ -5222,7 +5290,7 @@
         <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>411</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.2">
@@ -5230,7 +5298,7 @@
         <v>236</v>
       </c>
       <c r="E3" t="s">
-        <v>417</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.2">
@@ -5238,7 +5306,7 @@
         <v>387</v>
       </c>
       <c r="E4" t="s">
-        <v>417</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-9383 -updated dataset -created new keyword for splitting string and returning as a List
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6E0092-9049-4F42-AB46-021C9F181DEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6F6439-D3F1-465C-B441-D2E4D1F03448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="528">
   <si>
     <t>rowid</t>
   </si>
@@ -1616,6 +1616,12 @@
   </si>
   <si>
     <t>19Feb2021_CombineAndRollover</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>Delimiter</t>
   </si>
 </sst>
 </file>
@@ -4445,7 +4451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -4722,10 +4728,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4737,18 +4743,19 @@
     <col min="6" max="6" width="11.85546875" style="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="24" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
@@ -4773,35 +4780,38 @@
       <c r="H1" s="82" t="s">
         <v>436</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="I1" s="84" t="s">
+        <v>527</v>
+      </c>
+      <c r="J1" s="83" t="s">
         <v>404</v>
       </c>
-      <c r="J1" s="84" t="s">
+      <c r="K1" s="84" t="s">
         <v>437</v>
       </c>
-      <c r="K1" s="84" t="s">
+      <c r="L1" s="84" t="s">
         <v>438</v>
       </c>
-      <c r="L1" s="81" t="s">
+      <c r="M1" s="81" t="s">
         <v>439</v>
       </c>
-      <c r="M1" s="81" t="s">
+      <c r="N1" s="81" t="s">
         <v>440</v>
       </c>
-      <c r="N1" s="81" t="s">
+      <c r="O1" s="81" t="s">
         <v>406</v>
       </c>
-      <c r="O1" s="81" t="s">
+      <c r="P1" s="81" t="s">
         <v>441</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="Q1" s="64" t="s">
         <v>415</v>
       </c>
-      <c r="Q1" s="81" t="s">
+      <c r="R1" s="81" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>68</v>
       </c>
@@ -4824,29 +4834,30 @@
         <v>443</v>
       </c>
       <c r="H2" s="59"/>
-      <c r="I2" s="59" t="s">
+      <c r="I2" s="59"/>
+      <c r="J2" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="85" t="s">
+      <c r="K2" s="86"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="85" t="s">
         <v>444</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="N2" s="85" t="s">
         <v>445</v>
       </c>
-      <c r="N2" s="85" t="s">
+      <c r="O2" s="85" t="s">
         <v>225</v>
       </c>
-      <c r="O2" s="87" t="s">
+      <c r="P2" s="87" t="s">
         <v>429</v>
       </c>
-      <c r="P2" s="59" t="s">
+      <c r="Q2" s="59" t="s">
         <v>430</v>
       </c>
-      <c r="Q2" s="87"/>
+      <c r="R2" s="87"/>
     </row>
-    <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>236</v>
       </c>
@@ -4868,22 +4879,25 @@
         <f>_xlfn.CONCAT(G2,",",SERV01_LoanDrawdown!E3)</f>
         <v>60002220,60002225</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="24" t="s">
+        <v>526</v>
+      </c>
+      <c r="J3" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="85" t="s">
+      <c r="M3" s="85" t="s">
         <v>444</v>
       </c>
-      <c r="M3" s="85" t="s">
+      <c r="N3" s="85" t="s">
         <v>445</v>
       </c>
-      <c r="N3" s="85" t="s">
+      <c r="O3" s="85" t="s">
         <v>225</v>
       </c>
-      <c r="O3" s="87" t="s">
+      <c r="P3" s="87" t="s">
         <v>429</v>
       </c>
-      <c r="P3" s="90" t="s">
+      <c r="Q3" s="90" t="s">
         <v>430</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-9385 -updated dataset -new TC for March 19 2020 combine and rollover
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="4" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5535" yWindow="3555" windowWidth="21600" windowHeight="11385" tabRatio="877" firstSheet="4" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -3928,7 +3928,7 @@
   </sheetPr>
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -4440,10 +4440,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>19Feb2021_CombineAndRollover</t>
+          <t>19Feb2020_CombineAndRollover</t>
         </is>
       </c>
       <c r="C3" s="59" t="inlineStr">
@@ -4694,6 +4694,72 @@
         </is>
       </c>
       <c r="Q3" s="90" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1" s="24">
+      <c r="A4" s="25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" s="88" t="inlineStr">
+        <is>
+          <t>19Mar2020_CombineAndRollOver</t>
+        </is>
+      </c>
+      <c r="C4" s="59" t="inlineStr">
+        <is>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
+        </is>
+      </c>
+      <c r="E4" s="59" t="inlineStr">
+        <is>
+          <t>CLASS A DEBTHOLDERS17132</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>60002400</t>
+        </is>
+      </c>
+      <c r="H4">
+        <f>_xlfn.CONCAT(G3,",",SERV01_LoanDrawdown!E4)</f>
+        <v/>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="J4" s="59" t="inlineStr">
+        <is>
+          <t>NEW JB TRUST 1915659</t>
+        </is>
+      </c>
+      <c r="M4" s="85" t="inlineStr">
+        <is>
+          <t>Comprehensive Repricing</t>
+        </is>
+      </c>
+      <c r="N4" s="85" t="inlineStr">
+        <is>
+          <t>Rollover/Conversion to New:</t>
+        </is>
+      </c>
+      <c r="O4" s="85" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="P4" s="87" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+      <c r="Q4" s="90" t="inlineStr">
         <is>
           <t>Y</t>
         </is>

</xml_diff>

<commit_message>
GDE-9386 -updated data set -added new TC for collect commitment fee
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5535" yWindow="3555" windowWidth="21600" windowHeight="11385" tabRatio="877" firstSheet="4" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="4" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -3218,10 +3218,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI10"/>
+  <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3785,7 +3785,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" s="24">
       <c r="A7" s="25" t="inlineStr">
         <is>
           <t>6</t>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Amend_Commitment_Fee_19MAR2020</t>
+          <t>Collect_Commitment_Fee_19MAR2020</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">
@@ -3811,11 +3811,37 @@
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
-      <c r="M7" s="46" t="n"/>
+      <c r="H7" s="28" t="inlineStr">
+        <is>
+          <t>19-Mar-2020</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="M7" s="46" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="O7" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
+      </c>
+      <c r="Y7" t="n">
+        <v>-43599.73</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>117880745.28</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>365</v>
       </c>
     </row>
     <row r="8">
@@ -3826,7 +3852,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Amend_Commitment_Fee_20APR2020</t>
+          <t>Amend_Commitment_Fee_19MAR2020</t>
         </is>
       </c>
       <c r="C8" s="8" t="inlineStr">
@@ -3844,6 +3870,7 @@
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
+      <c r="M8" s="46" t="n"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
@@ -3858,7 +3885,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Amend_Commitment_Fee_19MAY2020</t>
+          <t>Amend_Commitment_Fee_20APR2020</t>
         </is>
       </c>
       <c r="C9" s="8" t="inlineStr">
@@ -3890,25 +3917,57 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Amend_Commitment_Fee_19MAY2020</t>
+        </is>
+      </c>
+      <c r="C10" s="8" t="inlineStr">
+        <is>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
+        </is>
+      </c>
+      <c r="D10" s="25" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="E10" s="8" t="inlineStr">
+        <is>
+          <t>CLASS A DEBTHOLDERS17132</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>NEW JB TRUST 1915659</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="25" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>Amend_Commitment_Fee_19JUN2020</t>
         </is>
       </c>
-      <c r="C10" s="8" t="inlineStr">
+      <c r="C11" s="8" t="inlineStr">
         <is>
           <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
         </is>
       </c>
-      <c r="D10" s="25" t="inlineStr">
+      <c r="D11" s="25" t="inlineStr">
         <is>
           <t>Commitment Fee</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E11" s="8" t="inlineStr">
         <is>
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -4442,7 +4501,7 @@
   </sheetPr>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GDE-9389 -updated dataset -added new tc for April 20 combine and rollover
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="8" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -4625,10 +4625,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4945,6 +4945,72 @@
         </is>
       </c>
       <c r="Q4" s="88" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1" s="23">
+      <c r="A5" s="24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>20Apr2020_CombineAndRollOver</t>
+        </is>
+      </c>
+      <c r="C5" s="58" t="inlineStr">
+        <is>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
+        </is>
+      </c>
+      <c r="E5" s="58" t="inlineStr">
+        <is>
+          <t>CLASS A DEBTHOLDERS17132</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>60002494</t>
+        </is>
+      </c>
+      <c r="H5">
+        <f>_xlfn.CONCAT(G4,",",SERV01_LoanDrawdown!E5)</f>
+        <v/>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="J5" s="58" t="inlineStr">
+        <is>
+          <t>NEW JB TRUST 1915659</t>
+        </is>
+      </c>
+      <c r="M5" s="83" t="inlineStr">
+        <is>
+          <t>Comprehensive Repricing</t>
+        </is>
+      </c>
+      <c r="N5" s="83" t="inlineStr">
+        <is>
+          <t>Rollover/Conversion to New:</t>
+        </is>
+      </c>
+      <c r="O5" s="83" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="P5" s="85" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+      <c r="Q5" s="88" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -5244,7 +5310,7 @@
   </sheetPr>
   <dimension ref="A1:BL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GDE-9390 -updated dataset -added tc for collect commitment fee
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5535" yWindow="3555" windowWidth="21600" windowHeight="11385" tabRatio="877" firstSheet="1" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -3218,10 +3218,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI11"/>
+  <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3483,11 +3483,7 @@
       </c>
       <c r="K2" s="27" t="n"/>
       <c r="L2" s="45" t="n"/>
-      <c r="M2" s="45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="M2" s="45" t="n"/>
       <c r="N2" s="45" t="n"/>
       <c r="O2" t="inlineStr">
         <is>
@@ -3557,11 +3553,7 @@
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
-      <c r="G3" s="27" t="inlineStr">
-        <is>
-          <t>13-Feb-2025</t>
-        </is>
-      </c>
+      <c r="G3" s="27" t="n"/>
       <c r="H3" s="27" t="inlineStr">
         <is>
           <t>19-Feb-2025</t>
@@ -3572,16 +3564,8 @@
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="J3" s="27" t="inlineStr">
-        <is>
-          <t>12-Feb-2025</t>
-        </is>
-      </c>
-      <c r="K3" s="27" t="inlineStr">
-        <is>
-          <t>Monthly</t>
-        </is>
-      </c>
+      <c r="J3" s="27" t="n"/>
+      <c r="K3" s="27" t="n"/>
       <c r="M3" s="45" t="inlineStr">
         <is>
           <t>1</t>
@@ -3619,6 +3603,11 @@
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
+      <c r="F4" s="27" t="inlineStr">
+        <is>
+          <t>16-Dec-2019</t>
+        </is>
+      </c>
       <c r="G4" s="27" t="inlineStr">
         <is>
           <t>13-Feb-2025</t>
@@ -3644,11 +3633,7 @@
           <t>Monthly</t>
         </is>
       </c>
-      <c r="M4" s="45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="M4" s="45" t="n"/>
       <c r="O4" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
@@ -3761,8 +3746,10 @@
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="J6" s="86" t="n">
-        <v>45731</v>
+      <c r="J6" s="27" t="inlineStr">
+        <is>
+          <t>15-Mar-2025</t>
+        </is>
       </c>
       <c r="K6" s="27" t="inlineStr">
         <is>
@@ -3900,47 +3887,75 @@
           <t>Monthly</t>
         </is>
       </c>
-      <c r="M8" s="45" t="inlineStr">
+      <c r="M8" s="45" t="n"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>NEW JB TRUST 1915659</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" s="23">
+      <c r="A9" s="24" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" s="89" t="inlineStr">
+        <is>
+          <t>Collect_Commitment_Fee_20APR2020</t>
+        </is>
+      </c>
+      <c r="C9" s="89" t="inlineStr">
+        <is>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
+        </is>
+      </c>
+      <c r="D9" s="24" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="E9" s="89" t="inlineStr">
+        <is>
+          <t>CLASS A DEBTHOLDERS17132</t>
+        </is>
+      </c>
+      <c r="G9" s="89" t="inlineStr">
+        <is>
+          <t>`</t>
+        </is>
+      </c>
+      <c r="H9" s="27" t="inlineStr">
+        <is>
+          <t>20-Apr-2020</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="M9" s="45" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="24" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Amend_Commitment_Fee_20APR2020</t>
-        </is>
-      </c>
-      <c r="C9" s="89" t="inlineStr">
-        <is>
-          <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
-        </is>
-      </c>
-      <c r="D9" s="24" t="inlineStr">
-        <is>
-          <t>Commitment Fee</t>
-        </is>
-      </c>
-      <c r="E9" s="89" t="inlineStr">
-        <is>
-          <t>CLASS A DEBTHOLDERS17132</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>NEW JB TRUST 1915659</t>
-        </is>
+      <c r="Y9" t="n">
+        <v>-132923.89</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>112830745.28</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>365</v>
       </c>
     </row>
     <row r="10">
@@ -3951,7 +3966,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Amend_Commitment_Fee_19MAY2020</t>
+          <t>Amend_Commitment_Fee_20APR2020</t>
         </is>
       </c>
       <c r="C10" s="89" t="inlineStr">
@@ -3983,25 +3998,57 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Amend_Commitment_Fee_19MAY2020</t>
+        </is>
+      </c>
+      <c r="C11" s="89" t="inlineStr">
+        <is>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
+        </is>
+      </c>
+      <c r="D11" s="24" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="E11" s="89" t="inlineStr">
+        <is>
+          <t>CLASS A DEBTHOLDERS17132</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>NEW JB TRUST 1915659</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="24" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>Amend_Commitment_Fee_19JUN2020</t>
         </is>
       </c>
-      <c r="C11" s="89" t="inlineStr">
+      <c r="C12" s="89" t="inlineStr">
         <is>
           <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
         </is>
       </c>
-      <c r="D11" s="24" t="inlineStr">
+      <c r="D12" s="24" t="inlineStr">
         <is>
           <t>Commitment Fee</t>
         </is>
       </c>
-      <c r="E11" s="89" t="inlineStr">
+      <c r="E12" s="89" t="inlineStr">
         <is>
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -4627,7 +4674,7 @@
   </sheetPr>
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GDE-9393 -updated dataset -added new tc collect commitment fee
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="1" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -3221,10 +3221,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI12"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Amend_Commitment_Fee_19MAY2020</t>
+          <t>Collect_Commitment_Fee_19MAY2020</t>
         </is>
       </c>
       <c r="C11" s="88" t="inlineStr">
@@ -4001,10 +4001,38 @@
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
+      <c r="F11" s="27" t="n"/>
+      <c r="H11" s="27" t="inlineStr">
+        <is>
+          <t>19-May-2020</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="M11" s="45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="O11" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
+      </c>
+      <c r="Y11" t="n">
+        <v>-236136.77</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>115691171.46</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>365</v>
       </c>
     </row>
     <row r="12">
@@ -4015,25 +4043,57 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Amend_Commitment_Fee_19MAY2020</t>
+        </is>
+      </c>
+      <c r="C12" s="88" t="inlineStr">
+        <is>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
+        </is>
+      </c>
+      <c r="D12" s="24" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="E12" s="88" t="inlineStr">
+        <is>
+          <t>CLASS A DEBTHOLDERS17132</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NEW JB TRUST 1915659</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="24" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>Amend_Commitment_Fee_19JUN2020</t>
         </is>
       </c>
-      <c r="C12" s="88" t="inlineStr">
+      <c r="C13" s="88" t="inlineStr">
         <is>
           <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
         </is>
       </c>
-      <c r="D12" s="24" t="inlineStr">
+      <c r="D13" s="24" t="inlineStr">
         <is>
           <t>Commitment Fee</t>
         </is>
       </c>
-      <c r="E12" s="88" t="inlineStr">
+      <c r="E13" s="88" t="inlineStr">
         <is>
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -4663,7 +4723,7 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GDE-9396 -updated data set -added new tc for collect commitment fee
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="877" firstSheet="2" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -3221,10 +3221,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AI14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4098,33 +4098,92 @@
         </is>
       </c>
     </row>
-    <row r="13">
+    <row r="13" s="23">
       <c r="A13" s="24" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="88" t="inlineStr">
+        <is>
+          <t>Collect_Commitment_Fee_19JUN2020</t>
+        </is>
+      </c>
+      <c r="C13" s="88" t="inlineStr">
+        <is>
+          <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
+        </is>
+      </c>
+      <c r="D13" s="24" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="E13" s="88" t="inlineStr">
+        <is>
+          <t>CLASS A DEBTHOLDERS17132</t>
+        </is>
+      </c>
+      <c r="H13" s="27" t="inlineStr">
+        <is>
+          <t>15-Jun-2020</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="M13" s="45" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>NEW JB TRUST 1915659</t>
+        </is>
+      </c>
+      <c r="Y13" t="n">
+        <v>-339149.46</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>115691171.46</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="24" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Amend_Commitment_Fee_19JUN2020</t>
         </is>
       </c>
-      <c r="C13" s="88" t="inlineStr">
+      <c r="C14" s="88" t="inlineStr">
         <is>
           <t>NEW LIFE BILAT AUD 320M 14FEB2018_05136</t>
         </is>
       </c>
-      <c r="D13" s="24" t="inlineStr">
+      <c r="D14" s="24" t="inlineStr">
         <is>
           <t>Commitment Fee</t>
         </is>
       </c>
-      <c r="E13" s="88" t="inlineStr">
+      <c r="E14" s="88" t="inlineStr">
         <is>
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -4754,8 +4813,8 @@
   </sheetPr>
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
GDE-9397 -updated dataset -added new locator for change expiry date window -added new keyword for change expiry date -added new tc
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -3221,10 +3221,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI14"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3235,25 +3235,25 @@
     <col width="28.85546875" bestFit="1" customWidth="1" style="23" min="5" max="5"/>
     <col width="26" bestFit="1" customWidth="1" style="23" min="6" max="6"/>
     <col width="23.85546875" bestFit="1" customWidth="1" style="23" min="7" max="7"/>
-    <col width="29.85546875" bestFit="1" customWidth="1" style="23" min="8" max="8"/>
-    <col width="20.140625" bestFit="1" customWidth="1" style="23" min="9" max="9"/>
-    <col width="28.5703125" bestFit="1" customWidth="1" style="23" min="10" max="10"/>
-    <col width="28.5703125" customWidth="1" style="23" min="11" max="11"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="23" min="12" max="12"/>
-    <col width="14.28515625" bestFit="1" customWidth="1" style="23" min="13" max="13"/>
-    <col width="12.85546875" bestFit="1" customWidth="1" style="23" min="14" max="14"/>
-    <col width="20.85546875" bestFit="1" customWidth="1" style="23" min="15" max="15"/>
-    <col width="22.140625" bestFit="1" customWidth="1" style="23" min="16" max="16"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="23" min="17" max="17"/>
-    <col width="10.42578125" bestFit="1" customWidth="1" style="23" min="18" max="18"/>
-    <col width="19.85546875" bestFit="1" customWidth="1" style="23" min="19" max="19"/>
-    <col width="29.42578125" bestFit="1" customWidth="1" style="23" min="21" max="21"/>
-    <col width="30.5703125" bestFit="1" customWidth="1" style="23" min="22" max="22"/>
-    <col width="20.140625" bestFit="1" customWidth="1" style="23" min="25" max="25"/>
-    <col width="16.5703125" bestFit="1" customWidth="1" style="23" min="27" max="27"/>
-    <col width="5.5703125" bestFit="1" customWidth="1" style="23" min="28" max="28"/>
-    <col width="10.85546875" bestFit="1" customWidth="1" style="23" min="29" max="29"/>
-    <col width="14" bestFit="1" customWidth="1" style="23" min="31" max="31"/>
+    <col width="29.85546875" bestFit="1" customWidth="1" style="23" min="8" max="9"/>
+    <col width="20.140625" bestFit="1" customWidth="1" style="23" min="10" max="10"/>
+    <col width="28.5703125" bestFit="1" customWidth="1" style="23" min="11" max="11"/>
+    <col width="28.5703125" customWidth="1" style="23" min="12" max="12"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="23" min="13" max="13"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" style="23" min="14" max="14"/>
+    <col width="12.85546875" bestFit="1" customWidth="1" style="23" min="15" max="15"/>
+    <col width="20.85546875" bestFit="1" customWidth="1" style="23" min="16" max="16"/>
+    <col width="22.140625" bestFit="1" customWidth="1" style="23" min="17" max="17"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="23" min="18" max="18"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" style="23" min="19" max="19"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="23" min="20" max="20"/>
+    <col width="29.42578125" bestFit="1" customWidth="1" style="23" min="22" max="22"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" style="23" min="23" max="23"/>
+    <col width="20.140625" bestFit="1" customWidth="1" style="23" min="26" max="26"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" style="23" min="28" max="28"/>
+    <col width="5.5703125" bestFit="1" customWidth="1" style="23" min="29" max="29"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" style="23" min="30" max="30"/>
+    <col width="14" bestFit="1" customWidth="1" style="23" min="32" max="32"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
@@ -3299,135 +3299,140 @@
       </c>
       <c r="I1" s="22" t="inlineStr">
         <is>
+          <t>Commitment_ExpiryDate</t>
+        </is>
+      </c>
+      <c r="J1" s="22" t="inlineStr">
+        <is>
           <t>Commitment_Accrue</t>
         </is>
       </c>
-      <c r="J1" s="22" t="inlineStr">
+      <c r="K1" s="22" t="inlineStr">
         <is>
           <t>Commitment_AccrualEndDate</t>
         </is>
       </c>
-      <c r="K1" s="22" t="inlineStr">
+      <c r="L1" s="22" t="inlineStr">
         <is>
           <t>Commitment_CycleFrequency</t>
         </is>
       </c>
-      <c r="L1" s="22" t="inlineStr">
+      <c r="M1" s="22" t="inlineStr">
         <is>
           <t>Payment_Type</t>
         </is>
       </c>
-      <c r="M1" s="22" t="inlineStr">
+      <c r="N1" s="22" t="inlineStr">
         <is>
           <t>Cycle_Number</t>
         </is>
       </c>
-      <c r="N1" s="22" t="inlineStr">
+      <c r="O1" s="22" t="inlineStr">
         <is>
           <t>Prorate_With</t>
         </is>
       </c>
-      <c r="O1" s="19" t="inlineStr">
+      <c r="P1" s="19" t="inlineStr">
         <is>
           <t>Borrower_ShortName</t>
         </is>
       </c>
-      <c r="P1" s="22" t="inlineStr">
+      <c r="Q1" s="22" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
       </c>
-      <c r="Q1" s="22" t="inlineStr">
+      <c r="R1" s="22" t="inlineStr">
         <is>
           <t>Remittance_Description</t>
         </is>
       </c>
-      <c r="R1" s="22" t="inlineStr">
+      <c r="S1" s="22" t="inlineStr">
         <is>
           <t>Host_Bank</t>
         </is>
       </c>
-      <c r="S1" s="22" t="inlineStr">
+      <c r="T1" s="22" t="inlineStr">
         <is>
           <t>Lender1_ShortName</t>
         </is>
       </c>
-      <c r="T1" s="22" t="inlineStr">
+      <c r="U1" s="22" t="inlineStr">
         <is>
           <t>Lender2_ShortName</t>
         </is>
       </c>
-      <c r="U1" s="47" t="inlineStr">
+      <c r="V1" s="47" t="inlineStr">
         <is>
           <t>Lender_RemittanceDescription</t>
         </is>
       </c>
-      <c r="V1" s="47" t="inlineStr">
+      <c r="W1" s="47" t="inlineStr">
         <is>
           <t>Lender2_RemittanceDescription</t>
         </is>
       </c>
-      <c r="W1" s="47" t="inlineStr">
+      <c r="X1" s="47" t="inlineStr">
         <is>
           <t>Lender_RemittanceInstruction</t>
         </is>
       </c>
-      <c r="X1" s="47" t="inlineStr">
+      <c r="Y1" s="47" t="inlineStr">
         <is>
           <t>Lender2_RemittanceInstruction</t>
         </is>
       </c>
-      <c r="Y1" s="19" t="inlineStr">
+      <c r="Z1" s="19" t="inlineStr">
         <is>
           <t>Computed_CycleDue</t>
         </is>
       </c>
-      <c r="Z1" s="19" t="inlineStr">
+      <c r="AA1" s="19" t="inlineStr">
         <is>
           <t>Rate</t>
         </is>
       </c>
-      <c r="AA1" s="19" t="inlineStr">
+      <c r="AB1" s="19" t="inlineStr">
         <is>
           <t>Balance_Amount</t>
         </is>
       </c>
-      <c r="AB1" s="19" t="inlineStr">
+      <c r="AC1" s="19" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="AC1" s="19" t="inlineStr">
+      <c r="AD1" s="19" t="inlineStr">
         <is>
           <t>Rate_Basis</t>
         </is>
       </c>
-      <c r="AD1" s="22" t="inlineStr">
+      <c r="AE1" s="22" t="inlineStr">
         <is>
           <t>Due_Date</t>
         </is>
       </c>
-      <c r="AE1" s="22" t="inlineStr">
+      <c r="AF1" s="22" t="inlineStr">
         <is>
           <t>Effective_Date</t>
         </is>
       </c>
-      <c r="AF1" s="22" t="inlineStr">
+      <c r="AG1" s="22" t="inlineStr">
         <is>
           <t>HostBankSharePct</t>
         </is>
       </c>
-      <c r="AG1" s="22" t="inlineStr">
+      <c r="AH1" s="22" t="inlineStr">
         <is>
           <t>LenderSharePct1</t>
         </is>
       </c>
-      <c r="AH1" s="22" t="inlineStr">
+      <c r="AI1" s="22" t="inlineStr">
         <is>
           <t>LenderSharePct2</t>
         </is>
       </c>
-      <c r="AI1" s="22" t="inlineStr">
+      <c r="AJ1" s="22" t="inlineStr">
         <is>
           <t>Fee_Cycle</t>
         </is>
@@ -3474,57 +3479,58 @@
           <t>21-Jan-2020</t>
         </is>
       </c>
-      <c r="I2" s="24" t="inlineStr">
+      <c r="I2" s="27" t="n"/>
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>to the adjusted due date</t>
         </is>
       </c>
-      <c r="J2" s="27" t="inlineStr">
+      <c r="K2" s="27" t="inlineStr">
         <is>
           <t>14-Jan-2020</t>
         </is>
       </c>
-      <c r="K2" s="27" t="inlineStr">
+      <c r="L2" s="27" t="inlineStr">
         <is>
           <t>Quarterly</t>
         </is>
       </c>
-      <c r="L2" s="45" t="n"/>
       <c r="M2" s="45" t="n"/>
       <c r="N2" s="45" t="n"/>
-      <c r="O2" t="inlineStr">
+      <c r="O2" s="45" t="n"/>
+      <c r="P2" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
       </c>
-      <c r="P2" s="58" t="inlineStr">
+      <c r="Q2" s="58" t="inlineStr">
         <is>
           <t>DDA</t>
         </is>
       </c>
-      <c r="Q2" s="65" t="inlineStr">
+      <c r="R2" s="65" t="inlineStr">
         <is>
           <t>DDA</t>
         </is>
       </c>
-      <c r="R2" s="43" t="n"/>
-      <c r="S2" s="49" t="n"/>
+      <c r="S2" s="43" t="n"/>
       <c r="T2" s="49" t="n"/>
-      <c r="U2" s="43" t="n"/>
+      <c r="U2" s="49" t="n"/>
       <c r="V2" s="43" t="n"/>
       <c r="W2" s="43" t="n"/>
       <c r="X2" s="43" t="n"/>
       <c r="Y2" s="43" t="n"/>
       <c r="Z2" s="43" t="n"/>
-      <c r="AA2" s="44" t="n"/>
-      <c r="AB2" s="43" t="n"/>
-      <c r="AC2" s="50" t="n"/>
-      <c r="AD2" s="45" t="n"/>
+      <c r="AA2" s="43" t="n"/>
+      <c r="AB2" s="44" t="n"/>
+      <c r="AC2" s="43" t="n"/>
+      <c r="AD2" s="50" t="n"/>
       <c r="AE2" s="45" t="n"/>
-      <c r="AF2" s="51" t="n"/>
+      <c r="AF2" s="45" t="n"/>
       <c r="AG2" s="51" t="n"/>
       <c r="AH2" s="51" t="n"/>
-      <c r="AI2" s="45" t="n"/>
+      <c r="AI2" s="51" t="n"/>
+      <c r="AJ2" s="45" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="24" t="inlineStr">
@@ -3558,19 +3564,20 @@
           <t>19-Feb-2020</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="27" t="n"/>
+      <c r="J3" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="J3" s="27" t="n"/>
       <c r="K3" s="27" t="n"/>
-      <c r="M3" s="45" t="inlineStr">
+      <c r="L3" s="27" t="n"/>
+      <c r="N3" s="45" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -3617,23 +3624,24 @@
           <t>19-Feb-2020</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="27" t="n"/>
+      <c r="J4" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="J4" s="27" t="inlineStr">
+      <c r="K4" s="27" t="inlineStr">
         <is>
           <t>12-Feb-2020</t>
         </is>
       </c>
-      <c r="K4" s="27" t="inlineStr">
+      <c r="L4" s="27" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="M4" s="45" t="n"/>
-      <c r="O4" t="inlineStr">
+      <c r="N4" s="45" t="n"/>
+      <c r="P4" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -3671,17 +3679,18 @@
           <t>19-Feb-2020</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="27" t="n"/>
+      <c r="J5" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="M5" s="45" t="inlineStr">
+      <c r="N5" s="45" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -3728,23 +3737,24 @@
           <t>19-Mar-2020</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" s="27" t="n"/>
+      <c r="J6" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="J6" s="27" t="inlineStr">
+      <c r="K6" s="27" t="inlineStr">
         <is>
           <t>15-Mar-2020</t>
         </is>
       </c>
-      <c r="K6" s="27" t="inlineStr">
+      <c r="L6" s="27" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="M6" s="45" t="n"/>
-      <c r="O6" t="inlineStr">
+      <c r="N6" s="45" t="n"/>
+      <c r="P6" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -3781,17 +3791,18 @@
           <t>19-Mar-2020</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="27" t="n"/>
+      <c r="J7" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="M7" s="45" t="inlineStr">
+      <c r="N7" s="45" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -3838,23 +3849,24 @@
           <t>20-Apr-2020</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" s="27" t="n"/>
+      <c r="J8" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="J8" s="27" t="inlineStr">
+      <c r="K8" s="27" t="inlineStr">
         <is>
           <t>14-Apr-2020</t>
         </is>
       </c>
-      <c r="K8" s="27" t="inlineStr">
+      <c r="L8" s="27" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="M8" s="45" t="n"/>
-      <c r="O8" t="inlineStr">
+      <c r="N8" s="45" t="n"/>
+      <c r="P8" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -3896,17 +3908,18 @@
           <t>20-Apr-2020</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" s="27" t="n"/>
+      <c r="J9" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="M9" s="45" t="inlineStr">
+      <c r="N9" s="45" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -3953,23 +3966,24 @@
           <t>19-May-2020</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="27" t="n"/>
+      <c r="J10" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="J10" s="27" t="inlineStr">
+      <c r="K10" s="27" t="inlineStr">
         <is>
           <t>13-May-2020</t>
         </is>
       </c>
-      <c r="K10" s="27" t="inlineStr">
+      <c r="L10" s="27" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="M10" s="45" t="n"/>
-      <c r="O10" t="inlineStr">
+      <c r="N10" s="45" t="n"/>
+      <c r="P10" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
@@ -4007,31 +4021,32 @@
           <t>19-May-2020</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" s="27" t="n"/>
+      <c r="J11" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="M11" s="45" t="inlineStr">
+      <c r="N11" s="45" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
       </c>
-      <c r="Y11" t="n">
+      <c r="Z11" t="n">
         <v>-236136.77</v>
       </c>
-      <c r="Z11" t="n">
+      <c r="AA11" t="n">
         <v>0.5</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AB11" t="n">
         <v>115691171.46</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AD11" t="n">
         <v>365</v>
       </c>
     </row>
@@ -4076,29 +4091,30 @@
           <t>19-Jun-2025</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" s="27" t="n"/>
+      <c r="J12" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="J12" s="27" t="inlineStr">
+      <c r="K12" s="27" t="inlineStr">
         <is>
           <t>15-Jun-2025</t>
         </is>
       </c>
-      <c r="K12" s="27" t="inlineStr">
+      <c r="L12" s="27" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="M12" s="45" t="n"/>
-      <c r="O12" t="inlineStr">
+      <c r="N12" s="45" t="n"/>
+      <c r="P12" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
       </c>
     </row>
-    <row r="13" s="23">
+    <row r="13">
       <c r="A13" s="24" t="inlineStr">
         <is>
           <t>12</t>
@@ -4129,38 +4145,39 @@
           <t>15-Jun-2020</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" s="27" t="n"/>
+      <c r="J13" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="M13" s="45" t="inlineStr">
+      <c r="N13" s="45" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
       </c>
-      <c r="Y13" t="n">
+      <c r="Z13" t="n">
         <v>-339149.46</v>
       </c>
-      <c r="Z13" t="n">
+      <c r="AA13" t="n">
         <v>0.5</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AB13" t="n">
         <v>115691171.46</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AD13" t="n">
         <v>365</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -4183,10 +4200,24 @@
           <t>CLASS A DEBTHOLDERS17132</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="I14" s="27" t="inlineStr">
+        <is>
+          <t>14-May-2020</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
         <is>
           <t>NEW JB TRUST 1915659</t>
         </is>
+      </c>
+      <c r="AA14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>115691171.46</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-9398 -applied review points -update data set
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBA1E03-ED68-45BE-A2B5-5DCEFA99EB15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581E8250-A4DC-46A2-BF21-899B288B759E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5880" yWindow="3900" windowWidth="21600" windowHeight="11385" tabRatio="877" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="574">
   <si>
     <t>rowid</t>
   </si>
@@ -1750,19 +1750,7 @@
     <t>EffectiveDate_FeePayment</t>
   </si>
   <si>
-    <t>EffectiveDate_Label</t>
-  </si>
-  <si>
-    <t>Window_name</t>
-  </si>
-  <si>
     <t>Reversal_Comment</t>
-  </si>
-  <si>
-    <t>Effective Date</t>
-  </si>
-  <si>
-    <t>Fee Reverse Fee</t>
   </si>
   <si>
     <t>Reverse Fee Payment (14/5/2020 - 16/6/2020)</t>
@@ -4144,10 +4132,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AP16"/>
+  <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1:AN1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4179,11 +4167,9 @@
     <col min="32" max="32" width="14" style="23" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="40" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -4293,25 +4279,19 @@
         <v>377</v>
       </c>
       <c r="AK1" s="37" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="AL1" s="37" t="s">
         <v>569</v>
       </c>
       <c r="AM1" s="37" t="s">
-        <v>570</v>
+        <v>548</v>
       </c>
       <c r="AN1" s="37" t="s">
-        <v>571</v>
-      </c>
-      <c r="AO1" s="37" t="s">
-        <v>548</v>
-      </c>
-      <c r="AP1" s="37" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
-    <row r="2" spans="1:42" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>68</v>
       </c>
@@ -4377,7 +4357,7 @@
       <c r="AI2" s="51"/>
       <c r="AJ2" s="45"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>236</v>
       </c>
@@ -4410,7 +4390,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>387</v>
       </c>
@@ -4450,7 +4430,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>235</v>
       </c>
@@ -4481,7 +4461,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>393</v>
       </c>
@@ -4521,7 +4501,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>398</v>
       </c>
@@ -4551,7 +4531,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>400</v>
       </c>
@@ -4591,7 +4571,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>405</v>
       </c>
@@ -4624,7 +4604,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>408</v>
       </c>
@@ -4664,7 +4644,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>232</v>
       </c>
@@ -4707,7 +4687,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>414</v>
       </c>
@@ -4747,7 +4727,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>419</v>
       </c>
@@ -4789,7 +4769,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>422</v>
       </c>
@@ -4821,7 +4801,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="87">
         <v>14</v>
       </c>
@@ -4844,33 +4824,25 @@
         <v>218</v>
       </c>
       <c r="AK15" s="88" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="AL15" s="24" t="s">
         <v>421</v>
       </c>
-      <c r="AM15" s="24" t="s">
+      <c r="AM15" s="92">
+        <v>3604.92</v>
+      </c>
+      <c r="AN15" s="23" t="s">
         <v>573</v>
       </c>
-      <c r="AN15" s="88" t="s">
-        <v>574</v>
-      </c>
-      <c r="AO15" s="92">
-        <v>3604.92</v>
-      </c>
-      <c r="AP15" s="23" t="s">
-        <v>577</v>
-      </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="AK16" s="23"/>
       <c r="AL16" s="23"/>
-      <c r="AM16" s="23"/>
+      <c r="AM16" s="93">
+        <v>52102.83</v>
+      </c>
       <c r="AN16" s="23"/>
-      <c r="AO16" s="93">
-        <v>52102.83</v>
-      </c>
-      <c r="AP16" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GDE-9399 -updated data set -added create ongoing fee button locator -added keyword for createing new ongoing fee
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_New_Life_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581E8250-A4DC-46A2-BF21-899B288B759E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEC6974-F0E5-49D2-B526-82592ED72901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="586">
   <si>
     <t>rowid</t>
   </si>
@@ -1760,6 +1760,42 @@
   </si>
   <si>
     <t>Fee Payment Released</t>
+  </si>
+  <si>
+    <t>ReversePayment19Jun2020</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16-Jun-2020</t>
+  </si>
+  <si>
+    <t>19-Jun-2020</t>
+  </si>
+  <si>
+    <t>CreateNewOngoingFee_19JUN2020</t>
+  </si>
+  <si>
+    <t>GLShortName</t>
+  </si>
+  <si>
+    <t>Special Acc't Pay.</t>
+  </si>
+  <si>
+    <t>UpfrontFee_EffectiveDate</t>
+  </si>
+  <si>
+    <t>13-Nov-2023</t>
+  </si>
+  <si>
+    <t>Needs to change to correct date</t>
+  </si>
+  <si>
+    <t>Needs to change to correct amount</t>
+  </si>
+  <si>
+    <t>3,604.92</t>
   </si>
 </sst>
 </file>
@@ -1966,7 +2002,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1998,6 +2034,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2005,7 +2054,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2194,6 +2243,9 @@
     </xf>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -3060,8 +3112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CV2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3591,7 +3643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -3847,7 +3899,7 @@
   <dimension ref="A1:AT3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4132,10 +4184,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AN16"/>
+  <dimension ref="A1:AR17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1:AN1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AQ16" sqref="AQ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4167,9 +4219,13 @@
     <col min="32" max="32" width="14" style="23" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="40" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -4290,8 +4346,20 @@
       <c r="AN1" s="37" t="s">
         <v>572</v>
       </c>
+      <c r="AO1" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="AP1" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="AQ1" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="AR1" s="22" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>68</v>
       </c>
@@ -4357,7 +4425,7 @@
       <c r="AI2" s="51"/>
       <c r="AJ2" s="45"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>236</v>
       </c>
@@ -4375,7 +4443,7 @@
       </c>
       <c r="G3" s="27"/>
       <c r="H3" s="27" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="I3" s="27"/>
       <c r="J3" t="s">
@@ -4390,7 +4458,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>387</v>
       </c>
@@ -4430,7 +4498,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>235</v>
       </c>
@@ -4461,7 +4529,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>393</v>
       </c>
@@ -4501,7 +4569,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>398</v>
       </c>
@@ -4531,7 +4599,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>400</v>
       </c>
@@ -4571,7 +4639,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>405</v>
       </c>
@@ -4604,7 +4672,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>408</v>
       </c>
@@ -4644,7 +4712,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>232</v>
       </c>
@@ -4687,7 +4755,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>414</v>
       </c>
@@ -4727,7 +4795,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>419</v>
       </c>
@@ -4769,7 +4837,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>422</v>
       </c>
@@ -4801,10 +4869,13 @@
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A15" s="87">
         <v>14</v>
       </c>
+      <c r="B15" s="23" t="s">
+        <v>574</v>
+      </c>
       <c r="C15" s="88" t="s">
         <v>213</v>
       </c>
@@ -4836,17 +4907,75 @@
         <v>573</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A16" s="87" t="s">
+        <v>575</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>578</v>
+      </c>
+      <c r="C16" s="88" t="s">
+        <v>213</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="E16" s="88" t="s">
+        <v>215</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>576</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>421</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>391</v>
+      </c>
       <c r="AK16" s="23"/>
       <c r="AL16" s="23"/>
       <c r="AM16" s="93">
         <v>52102.83</v>
       </c>
       <c r="AN16" s="23"/>
+      <c r="AO16" s="94" t="s">
+        <v>580</v>
+      </c>
+      <c r="AP16" s="24" t="s">
+        <v>582</v>
+      </c>
+      <c r="AQ16" s="87" t="s">
+        <v>585</v>
+      </c>
+      <c r="AR16" s="88" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A17" s="87"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="88"/>
+      <c r="H17" s="27"/>
+      <c r="AP17" t="s">
+        <v>583</v>
+      </c>
+      <c r="AQ17" s="23" t="s">
+        <v>584</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5247,7 +5376,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>